<commit_message>
Updated data model to implement UTC_TZ_OFFSET field.  Updated leg template and load_ref_data.sql to include SE-19-06
</commit_message>
<xml_diff>
--- a/docs/Cruise_Leg_DDL_DML_generator.xlsx
+++ b/docs/Cruise_Leg_DDL_DML_generator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="32" activeTab="35"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Vessels" sheetId="10" r:id="rId1"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4818" uniqueCount="2018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4953" uniqueCount="2026">
   <si>
     <t>Cruise Name</t>
   </si>
@@ -6192,6 +6192,30 @@
   </si>
   <si>
     <t>RL-17-05 Leg 6</t>
+  </si>
+  <si>
+    <t>SE-19-06</t>
+  </si>
+  <si>
+    <t>Created MOUSS cruise so it can be referenced by the MOUSS database</t>
+  </si>
+  <si>
+    <t>9/11/2019</t>
+  </si>
+  <si>
+    <t>9/29/2019</t>
+  </si>
+  <si>
+    <t>Leg dates retrieved from project report</t>
+  </si>
+  <si>
+    <t>SE1906</t>
+  </si>
+  <si>
+    <t>UTC_TZ_OFFSET</t>
+  </si>
+  <si>
+    <t>-10:00</t>
   </si>
 </sst>
 </file>
@@ -25706,8 +25730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView topLeftCell="B67" workbookViewId="0">
-      <selection activeCell="L82" sqref="L82:L102"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25833,7 +25857,7 @@
         <v>1868</v>
       </c>
       <c r="L3" s="2" t="str">
-        <f t="shared" ref="L3:L51" si="0">CONCATENATE("insert into ccd_cruises (cruise_name, cruise_notes, sci_center_div_id, std_svy_name_id, svy_freq_id, std_svy_name_oth, CRUISE_URL, CRUISE_CONT_EMAIL, svy_type_id, CRUISE_DESC, OBJ_BASED_METRICS) values ('", A3, "', '", SUBSTITUTE(C3, "'", "''"), "', (select sci_center_div_id from ccd_sci_center_divs where sci_center_div_code = '", SUBSTITUTE(E3, "'", "''"),"'), (select STD_SVY_NAME_ID from ccd_std_svy_names where std_svy_name = '", SUBSTITUTE(D3, "'", "''"), "'), (select SVY_FREQ_ID from ccd_svy_freq where SVY_FREQ_name = '", SUBSTITUTE(F3, "'", "''"), "'), (CASE WHEN (select STD_SVY_NAME_ID from ccd_std_svy_names where std_svy_name = '", SUBSTITUTE(D3, "'", "''"), "') IS NULL THEN '", SUBSTITUTE(D3, "'", "''"), "' ELSE NULL END), '", SUBSTITUTE(G3, "'", "''"), "', '", SUBSTITUTE(H3, "'", "''"), "', (SELECT svy_type_id from ccd_svy_types where svy_type_name = '", SUBSTITUTE(I3, "'", "''"), "'), '", SUBSTITUTE(J3, "'", "''"), "', '", SUBSTITUTE(K3, "'", "''"), "');")</f>
+        <f t="shared" ref="L3:L52" si="0">CONCATENATE("insert into ccd_cruises (cruise_name, cruise_notes, sci_center_div_id, std_svy_name_id, svy_freq_id, std_svy_name_oth, CRUISE_URL, CRUISE_CONT_EMAIL, svy_type_id, CRUISE_DESC, OBJ_BASED_METRICS) values ('", A3, "', '", SUBSTITUTE(C3, "'", "''"), "', (select sci_center_div_id from ccd_sci_center_divs where sci_center_div_code = '", SUBSTITUTE(E3, "'", "''"),"'), (select STD_SVY_NAME_ID from ccd_std_svy_names where std_svy_name = '", SUBSTITUTE(D3, "'", "''"), "'), (select SVY_FREQ_ID from ccd_svy_freq where SVY_FREQ_name = '", SUBSTITUTE(F3, "'", "''"), "'), (CASE WHEN (select STD_SVY_NAME_ID from ccd_std_svy_names where std_svy_name = '", SUBSTITUTE(D3, "'", "''"), "') IS NULL THEN '", SUBSTITUTE(D3, "'", "''"), "' ELSE NULL END), '", SUBSTITUTE(G3, "'", "''"), "', '", SUBSTITUTE(H3, "'", "''"), "', (SELECT svy_type_id from ccd_svy_types where svy_type_name = '", SUBSTITUTE(I3, "'", "''"), "'), '", SUBSTITUTE(J3, "'", "''"), "', '", SUBSTITUTE(K3, "'", "''"), "');")</f>
         <v>insert into ccd_cruises (cruise_name, cruise_notes, sci_center_div_id, std_svy_name_id, svy_freq_id, std_svy_name_oth, CRUISE_URL, CRUISE_CONT_EMAIL, svy_type_id, CRUISE_DESC, OBJ_BASED_METRICS) values ('HA1008', 'Retrieved this information manually from FINSS on 1/16/20 for testing purposes', (select sci_center_div_id from ccd_sci_center_divs where sci_center_div_code = 'ESD'), (select STD_SVY_NAME_ID from ccd_std_svy_names where std_svy_name = 'Coral Reef Ecosystem Research'), (select SVY_FREQ_ID from ccd_svy_freq where SVY_FREQ_name = 'ANNUAL'), (CASE WHEN (select STD_SVY_NAME_ID from ccd_std_svy_names where std_svy_name = 'Coral Reef Ecosystem Research') IS NULL THEN 'Coral Reef Ecosystem Research' ELSE NULL END), 'http://www.noaa.gov/testURL', 'test@test.com', (SELECT svy_type_id from ccd_svy_types where svy_type_name = 'NMFS Survey'), 'Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.', 'test content');</v>
       </c>
     </row>
@@ -27638,6 +27662,45 @@
       <c r="L51" s="2" t="str">
         <f t="shared" si="0"/>
         <v>insert into ccd_cruises (cruise_name, cruise_notes, sci_center_div_id, std_svy_name_id, svy_freq_id, std_svy_name_oth, CRUISE_URL, CRUISE_CONT_EMAIL, svy_type_id, CRUISE_DESC, OBJ_BASED_METRICS) values ('SE-18-03', 'Retrieved this information manually from FINSS on 1/16/20 for testing purposes', (select sci_center_div_id from ccd_sci_center_divs where sci_center_div_code = 'PSD'), (select STD_SVY_NAME_ID from ccd_std_svy_names where std_svy_name = 'Mariana Archipelago Cetacean Survey (MACS)'), (select SVY_FREQ_ID from ccd_svy_freq where SVY_FREQ_name = 'ANNUAL'), (CASE WHEN (select STD_SVY_NAME_ID from ccd_std_svy_names where std_svy_name = 'Mariana Archipelago Cetacean Survey (MACS)') IS NULL THEN 'Mariana Archipelago Cetacean Survey (MACS)' ELSE NULL END), 'http://www.noaa.gov/testURL', 'test@test.com', (SELECT svy_type_id from ccd_svy_types where svy_type_name = 'NMFS Survey'), 'Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.', 'test content');</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>2018</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>2019</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>1861</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>1421</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>1763</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>1762</v>
+      </c>
+      <c r="I52" t="s">
+        <v>1715</v>
+      </c>
+      <c r="J52" t="s">
+        <v>1867</v>
+      </c>
+      <c r="K52" t="s">
+        <v>1868</v>
+      </c>
+      <c r="L52" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruises (cruise_name, cruise_notes, sci_center_div_id, std_svy_name_id, svy_freq_id, std_svy_name_oth, CRUISE_URL, CRUISE_CONT_EMAIL, svy_type_id, CRUISE_DESC, OBJ_BASED_METRICS) values ('SE-19-06', 'Created MOUSS cruise so it can be referenced by the MOUSS database', (select sci_center_div_id from ccd_sci_center_divs where sci_center_div_code = 'FRMD'), (select STD_SVY_NAME_ID from ccd_std_svy_names where std_svy_name = 'Hawaiian Archipelago Insular Bottomfish Survey'), (select SVY_FREQ_ID from ccd_svy_freq where SVY_FREQ_name = 'ANNUAL'), (CASE WHEN (select STD_SVY_NAME_ID from ccd_std_svy_names where std_svy_name = 'Hawaiian Archipelago Insular Bottomfish Survey') IS NULL THEN 'Hawaiian Archipelago Insular Bottomfish Survey' ELSE NULL END), 'http://www.noaa.gov/testURL', 'test@test.com', (SELECT svy_type_id from ccd_svy_types where svy_type_name = 'NMFS Survey'), 'Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.', 'test content');</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -28843,9 +28906,11 @@
     <hyperlink ref="H102" r:id="rId40"/>
     <hyperlink ref="G101" r:id="rId41"/>
     <hyperlink ref="G102" r:id="rId42"/>
+    <hyperlink ref="G52" r:id="rId43"/>
+    <hyperlink ref="H52" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId43"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId45"/>
 </worksheet>
 </file>
 
@@ -43178,11 +43243,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H121"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A86" sqref="A86:XFD89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I69" sqref="I2:I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43190,10 +43255,10 @@
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="65.5703125" customWidth="1"/>
-    <col min="6" max="7" width="19.7109375" customWidth="1"/>
+    <col min="6" max="8" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1717</v>
       </c>
@@ -43216,10 +43281,13 @@
         <v>1725</v>
       </c>
       <c r="H1" t="s">
+        <v>2024</v>
+      </c>
+      <c r="I1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -43238,12 +43306,15 @@
       <c r="G2" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H2" s="5" t="str">
-        <f>CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ") values ('", SUBSTITUTE(B2, "'", "''"), "', TO_DATE('", C2, "', 'MM/DD/YYYY'), TO_DATE('", D2, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E2, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F2, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A2, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G2, "'", "''"), "'));")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-17-07', TO_DATE('10/20/2017', 'MM/DD/YYYY'), TO_DATE('11/03/2017', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-07'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I2" s="5" t="str">
+        <f>CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B2, "'", "''"), "', TO_DATE('", C2, "', 'MM/DD/YYYY'), TO_DATE('", D2, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E2, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F2, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A2, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G2, "'", "''"), "'), '", H2, "');")</f>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-17-07', TO_DATE('10/20/2017', 'MM/DD/YYYY'), TO_DATE('11/03/2017', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-07'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -43262,12 +43333,15 @@
       <c r="G3" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H3" s="5" t="str">
-        <f t="shared" ref="H3:H66" si="0">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ") values ('", SUBSTITUTE(B3, "'", "''"), "', TO_DATE('", C3, "', 'MM/DD/YYYY'), TO_DATE('", D3, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E3, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F3, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A3, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G3, "'", "''"), "'));")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-18-06', TO_DATE('10/17/2018', 'MM/DD/YYYY'), TO_DATE('10/31/2018', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-18-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I3" s="5" t="str">
+        <f t="shared" ref="I3:I66" si="0">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B3, "'", "''"), "', TO_DATE('", C3, "', 'MM/DD/YYYY'), TO_DATE('", D3, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E3, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F3, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A3, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G3, "'", "''"), "'), '", H3, "');")</f>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-18-06', TO_DATE('10/17/2018', 'MM/DD/YYYY'), TO_DATE('10/31/2018', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-18-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -43286,12 +43360,15 @@
       <c r="G4" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H4" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-17-02', TO_DATE('3/1/2017', 'MM/DD/YYYY'), TO_DATE('3/15/2017', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-17-02', TO_DATE('3/1/2017', 'MM/DD/YYYY'), TO_DATE('3/15/2017', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -43310,12 +43387,15 @@
       <c r="G5" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H5" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-15-01', TO_DATE('4/3/2015', 'MM/DD/YYYY'), TO_DATE('4/14/2015', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-15-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I5" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-15-01', TO_DATE('4/3/2015', 'MM/DD/YYYY'), TO_DATE('4/14/2015', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-15-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -43334,12 +43414,15 @@
       <c r="G6" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H6" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HA1201_LEG_I', TO_DATE('2/27/2012', 'MM/DD/YYYY'), TO_DATE('3/25/2012', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1201'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I6" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HA1201_LEG_I', TO_DATE('2/27/2012', 'MM/DD/YYYY'), TO_DATE('3/25/2012', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1201'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -43358,12 +43441,15 @@
       <c r="G7" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H7" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HA1201_LEG_II&amp;III', TO_DATE('4/1/2012', 'MM/DD/YYYY'), TO_DATE('4/27/2012', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1201'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I7" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HA1201_LEG_II&amp;III', TO_DATE('4/1/2012', 'MM/DD/YYYY'), TO_DATE('4/27/2012', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1201'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -43382,12 +43468,15 @@
       <c r="G8" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H8" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HA1201_LEG_IV', TO_DATE('4/27/2012', 'MM/DD/YYYY'), TO_DATE('5/24/2012', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1201'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I8" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HA1201_LEG_IV', TO_DATE('4/27/2012', 'MM/DD/YYYY'), TO_DATE('5/24/2012', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1201'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -43406,12 +43495,15 @@
       <c r="G9" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H9" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HA1101_LEG_I', TO_DATE('3/10/2011', 'MM/DD/YYYY'), TO_DATE('4/5/2011', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1101'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I9" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HA1101_LEG_I', TO_DATE('3/10/2011', 'MM/DD/YYYY'), TO_DATE('4/5/2011', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1101'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -43430,12 +43522,15 @@
       <c r="G10" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H10" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HA1101_LEG_II', TO_DATE('4/7/2011', 'MM/DD/YYYY'), TO_DATE('5/9/2011', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1101'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I10" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HA1101_LEG_II', TO_DATE('4/7/2011', 'MM/DD/YYYY'), TO_DATE('5/9/2011', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1101'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -43454,12 +43549,15 @@
       <c r="G11" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H11" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HA1101_LEG_III', TO_DATE('5/12/2011', 'MM/DD/YYYY'), TO_DATE('5/24/2011', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1101'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I11" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HA1101_LEG_III', TO_DATE('5/12/2011', 'MM/DD/YYYY'), TO_DATE('5/24/2011', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1101'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -43478,12 +43576,15 @@
       <c r="G12" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H12" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HA1007', TO_DATE('9/4/2010', 'MM/DD/YYYY'), TO_DATE('9/29/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1007'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I12" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HA1007', TO_DATE('9/4/2010', 'MM/DD/YYYY'), TO_DATE('9/29/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1007'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -43502,12 +43603,15 @@
       <c r="G13" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H13" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HA1008', TO_DATE('10/7/2010', 'MM/DD/YYYY'), TO_DATE('11/5/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1008'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I13" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HA1008', TO_DATE('10/7/2010', 'MM/DD/YYYY'), TO_DATE('11/5/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1008'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -43526,12 +43630,15 @@
       <c r="G14" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H14" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI0401', TO_DATE('9/13/2004', 'MM/DD/YYYY'), TO_DATE('10/17/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0401'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I14" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI0401', TO_DATE('9/13/2004', 'MM/DD/YYYY'), TO_DATE('10/17/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0401'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -43550,12 +43657,15 @@
       <c r="G15" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H15" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI0602', TO_DATE('2/9/2006', 'MM/DD/YYYY'), TO_DATE('3/10/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0602'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I15" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI0602', TO_DATE('2/9/2006', 'MM/DD/YYYY'), TO_DATE('3/10/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0602'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -43574,12 +43684,15 @@
       <c r="G16" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H16" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI0604', TO_DATE('3/15/2006', 'MM/DD/YYYY'), TO_DATE('4/8/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0604'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I16" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI0604', TO_DATE('3/15/2006', 'MM/DD/YYYY'), TO_DATE('4/8/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0604'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -43598,12 +43711,15 @@
       <c r="G17" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H17" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI0609', TO_DATE('6/23/2006', 'MM/DD/YYYY'), TO_DATE('7/20/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0609'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I17" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI0609', TO_DATE('6/23/2006', 'MM/DD/YYYY'), TO_DATE('7/20/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0609'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -43622,12 +43738,15 @@
       <c r="G18" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H18" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI0610', TO_DATE('7/27/2006', 'MM/DD/YYYY'), TO_DATE('8/20/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0610'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI0610', TO_DATE('7/27/2006', 'MM/DD/YYYY'), TO_DATE('8/20/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0610'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -43646,12 +43765,15 @@
       <c r="G19" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H19" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI0611', TO_DATE('9/1/2006', 'MM/DD/YYYY'), TO_DATE('10/4/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0611'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I19" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI0611', TO_DATE('9/1/2006', 'MM/DD/YYYY'), TO_DATE('10/4/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0611'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -43670,12 +43792,15 @@
       <c r="G20" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H20" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI0701', TO_DATE('4/19/2007', 'MM/DD/YYYY'), TO_DATE('5/9/2007', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0701'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I20" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI0701', TO_DATE('4/19/2007', 'MM/DD/YYYY'), TO_DATE('5/9/2007', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0701'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -43694,12 +43819,15 @@
       <c r="G21" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H21" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI1001_LEGI', TO_DATE('1/21/2010', 'MM/DD/YYYY'), TO_DATE('2/14/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1001'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I21" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI1001_LEGI', TO_DATE('1/21/2010', 'MM/DD/YYYY'), TO_DATE('2/14/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1001'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -43718,12 +43846,15 @@
       <c r="G22" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H22" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI1001_LEGII', TO_DATE('2/17/2010', 'MM/DD/YYYY'), TO_DATE('3/23/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1001'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I22" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI1001_LEGII', TO_DATE('2/17/2010', 'MM/DD/YYYY'), TO_DATE('3/23/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1001'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -43742,12 +43873,15 @@
       <c r="G23" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H23" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI1001_LEGIII', TO_DATE('3/27/2010', 'MM/DD/YYYY'), TO_DATE('4/24/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1001'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I23" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI1001_LEGIII', TO_DATE('3/27/2010', 'MM/DD/YYYY'), TO_DATE('4/24/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1001'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -43766,12 +43900,15 @@
       <c r="G24" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H24" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0304', TO_DATE('5/13/2003', 'MM/DD/YYYY'), TO_DATE('5/28/2003', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0304'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I24" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0304', TO_DATE('5/13/2003', 'MM/DD/YYYY'), TO_DATE('5/28/2003', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0304'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -43790,12 +43927,15 @@
       <c r="G25" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H25" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0306', TO_DATE('7/12/2003', 'MM/DD/YYYY'), TO_DATE('8/17/2003', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0306'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I25" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0306', TO_DATE('7/12/2003', 'MM/DD/YYYY'), TO_DATE('8/17/2003', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0306'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -43814,12 +43954,15 @@
       <c r="G26" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H26" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0407', TO_DATE('5/30/2004', 'MM/DD/YYYY'), TO_DATE('6/14/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0407'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I26" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0407', TO_DATE('5/30/2004', 'MM/DD/YYYY'), TO_DATE('6/14/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0407'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -43838,12 +43981,15 @@
       <c r="G27" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H27" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0410', TO_DATE('7/30/2004', 'MM/DD/YYYY'), TO_DATE('8/16/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0410'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H27" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I27" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0410', TO_DATE('7/30/2004', 'MM/DD/YYYY'), TO_DATE('8/16/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0410'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -43862,12 +44008,15 @@
       <c r="G28" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H28" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0411_LEGI', TO_DATE('8/7/2004', 'MM/DD/YYYY'), TO_DATE('9/7/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0411'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I28" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0411_LEGI', TO_DATE('8/7/2004', 'MM/DD/YYYY'), TO_DATE('9/7/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0411'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -43886,12 +44035,15 @@
       <c r="G29" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H29" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0411_LEGII', TO_DATE('9/8/2004', 'MM/DD/YYYY'), TO_DATE('9/13/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0411'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I29" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0411_LEGII', TO_DATE('9/8/2004', 'MM/DD/YYYY'), TO_DATE('9/13/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0411'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -43910,12 +44062,15 @@
       <c r="G30" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H30" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0504', TO_DATE('3/21/2005', 'MM/DD/YYYY'), TO_DATE('4/3/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0504'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I30" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0504', TO_DATE('3/21/2005', 'MM/DD/YYYY'), TO_DATE('4/3/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0504'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -43934,12 +44089,15 @@
       <c r="G31" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H31" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0506', TO_DATE('5/5/2005', 'MM/DD/YYYY'), TO_DATE('5/20/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0506'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I31" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0506', TO_DATE('5/5/2005', 'MM/DD/YYYY'), TO_DATE('5/20/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0506'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -43958,12 +44116,15 @@
       <c r="G32" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H32" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0509', TO_DATE('7/19/2005', 'MM/DD/YYYY'), TO_DATE('8/5/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0509'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H32" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I32" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0509', TO_DATE('7/19/2005', 'MM/DD/YYYY'), TO_DATE('8/5/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0509'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -43982,12 +44143,15 @@
       <c r="G33" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H33" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0512', TO_DATE('10/3/2005', 'MM/DD/YYYY'), TO_DATE('10/9/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0512'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I33" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0512', TO_DATE('10/3/2005', 'MM/DD/YYYY'), TO_DATE('10/9/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0512'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -44006,12 +44170,15 @@
       <c r="G34" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H34" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0604', TO_DATE('4/6/2006', 'MM/DD/YYYY'), TO_DATE('4/17/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0604'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I34" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0604', TO_DATE('4/6/2006', 'MM/DD/YYYY'), TO_DATE('4/17/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0604'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -44030,12 +44197,15 @@
       <c r="G35" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H35" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0606', TO_DATE('5/8/2006', 'MM/DD/YYYY'), TO_DATE('5/23/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0606'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H35" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I35" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0606', TO_DATE('5/8/2006', 'MM/DD/YYYY'), TO_DATE('5/23/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0606'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -44054,12 +44224,15 @@
       <c r="G36" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H36" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0607', TO_DATE('6/5/2006', 'MM/DD/YYYY'), TO_DATE('7/3/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0607'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I36" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0607', TO_DATE('6/5/2006', 'MM/DD/YYYY'), TO_DATE('7/3/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0607'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -44078,12 +44251,15 @@
       <c r="G37" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H37" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0608', TO_DATE('7/17/2006', 'MM/DD/YYYY'), TO_DATE('8/3/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0608'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H37" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I37" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0608', TO_DATE('7/17/2006', 'MM/DD/YYYY'), TO_DATE('8/3/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0608'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -44102,12 +44278,15 @@
       <c r="G38" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H38" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0706', TO_DATE('7/18/2007', 'MM/DD/YYYY'), TO_DATE('8/14/2007', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0706'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I38" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0706', TO_DATE('7/18/2007', 'MM/DD/YYYY'), TO_DATE('8/14/2007', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0706'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -44126,12 +44305,15 @@
       <c r="G39" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H39" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0908_LEGI', TO_DATE('9/1/2009', 'MM/DD/YYYY'), TO_DATE('9/30/2009', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0908'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I39" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0908_LEGI', TO_DATE('9/1/2009', 'MM/DD/YYYY'), TO_DATE('9/30/2009', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0908'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -44150,12 +44332,15 @@
       <c r="G40" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H40" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('OES0908_LEGII', TO_DATE('10/6/2009', 'MM/DD/YYYY'), TO_DATE('10/30/2009', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0908'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I40" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0908_LEGII', TO_DATE('10/6/2009', 'MM/DD/YYYY'), TO_DATE('10/30/2009', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0908'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -44174,12 +44359,15 @@
       <c r="G41" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H41" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC0009', TO_DATE('7/19/2000', 'MM/DD/YYYY'), TO_DATE('8/4/2000', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0009'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I41" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0009', TO_DATE('7/19/2000', 'MM/DD/YYYY'), TO_DATE('8/4/2000', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0009'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>79</v>
       </c>
@@ -44198,12 +44386,15 @@
       <c r="G42" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H42" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC0011', TO_DATE('9/8/2000', 'MM/DD/YYYY'), TO_DATE('10/6/2000', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0011'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I42" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0011', TO_DATE('9/8/2000', 'MM/DD/YYYY'), TO_DATE('10/6/2000', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0011'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -44222,12 +44413,15 @@
       <c r="G43" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H43" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC0012', TO_DATE('10/9/2000', 'MM/DD/YYYY'), TO_DATE('11/5/2000', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0012'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H43" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I43" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0012', TO_DATE('10/9/2000', 'MM/DD/YYYY'), TO_DATE('11/5/2000', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0012'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -44246,12 +44440,15 @@
       <c r="G44" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H44" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC0108', TO_DATE('7/16/2001', 'MM/DD/YYYY'), TO_DATE('8/2/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0108'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I44" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0108', TO_DATE('7/16/2001', 'MM/DD/YYYY'), TO_DATE('8/2/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0108'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>79</v>
       </c>
@@ -44270,12 +44467,15 @@
       <c r="G45" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H45" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC0109_LEGI', TO_DATE('8/7/2001', 'MM/DD/YYYY'), TO_DATE('8/11/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0109'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H45" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I45" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0109_LEGI', TO_DATE('8/7/2001', 'MM/DD/YYYY'), TO_DATE('8/11/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0109'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>79</v>
       </c>
@@ -44294,12 +44494,15 @@
       <c r="G46" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H46" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC0109_LEGII', TO_DATE('8/12/2001', 'MM/DD/YYYY'), TO_DATE('8/27/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0109'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H46" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I46" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0109_LEGII', TO_DATE('8/12/2001', 'MM/DD/YYYY'), TO_DATE('8/27/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0109'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>79</v>
       </c>
@@ -44318,12 +44521,15 @@
       <c r="G47" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H47" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC0110', TO_DATE('9/10/2001', 'MM/DD/YYYY'), TO_DATE('10/1/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0110'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H47" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I47" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0110', TO_DATE('9/10/2001', 'MM/DD/YYYY'), TO_DATE('10/1/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0110'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>79</v>
       </c>
@@ -44342,12 +44548,15 @@
       <c r="G48" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H48" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC0111', TO_DATE('10/22/2001', 'MM/DD/YYYY'), TO_DATE('11/20/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0111'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H48" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I48" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0111', TO_DATE('10/22/2001', 'MM/DD/YYYY'), TO_DATE('11/20/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0111'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>79</v>
       </c>
@@ -44366,12 +44575,15 @@
       <c r="G49" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H49" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC0201_LEGI', TO_DATE('1/21/2002', 'MM/DD/YYYY'), TO_DATE('3/25/2002', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0201'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H49" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I49" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0201_LEGI', TO_DATE('1/21/2002', 'MM/DD/YYYY'), TO_DATE('3/25/2002', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0201'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -44390,12 +44602,15 @@
       <c r="G50" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H50" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC0201_LEGII', TO_DATE('1/21/2002', 'MM/DD/YYYY'), TO_DATE('3/25/2002', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0201'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H50" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I50" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0201_LEGII', TO_DATE('1/21/2002', 'MM/DD/YYYY'), TO_DATE('3/25/2002', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0201'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>79</v>
       </c>
@@ -44414,12 +44629,15 @@
       <c r="G51" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H51" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC0207', TO_DATE('9/8/2002', 'MM/DD/YYYY'), TO_DATE('10/7/2002', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0207'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H51" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I51" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0207', TO_DATE('9/8/2002', 'MM/DD/YYYY'), TO_DATE('10/7/2002', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0207'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -44438,12 +44656,15 @@
       <c r="G52" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H52" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC9905', TO_DATE('4/26/1999', 'MM/DD/YYYY'), TO_DATE('5/9/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9905'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H52" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I52" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC9905', TO_DATE('4/26/1999', 'MM/DD/YYYY'), TO_DATE('5/9/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9905'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>79</v>
       </c>
@@ -44462,12 +44683,15 @@
       <c r="G53" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H53" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC9906', TO_DATE('5/15/1999', 'MM/DD/YYYY'), TO_DATE('5/31/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9906'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H53" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I53" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC9906', TO_DATE('5/15/1999', 'MM/DD/YYYY'), TO_DATE('5/31/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9906'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>79</v>
       </c>
@@ -44486,12 +44710,15 @@
       <c r="G54" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H54" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC9908', TO_DATE('7/15/1999', 'MM/DD/YYYY'), TO_DATE('8/2/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9908'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H54" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I54" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC9908', TO_DATE('7/15/1999', 'MM/DD/YYYY'), TO_DATE('8/2/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9908'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>79</v>
       </c>
@@ -44510,12 +44737,15 @@
       <c r="G55" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H55" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC9909_LEGI', TO_DATE('8/13/1999', 'MM/DD/YYYY'), TO_DATE('8/29/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9909'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H55" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I55" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC9909_LEGI', TO_DATE('8/13/1999', 'MM/DD/YYYY'), TO_DATE('8/29/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9909'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>79</v>
       </c>
@@ -44534,12 +44764,15 @@
       <c r="G56" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H56" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC9909_LEGII', TO_DATE('8/30/1999', 'MM/DD/YYYY'), TO_DATE('9/7/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9909'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H56" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I56" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC9909_LEGII', TO_DATE('8/30/1999', 'MM/DD/YYYY'), TO_DATE('9/7/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9909'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>79</v>
       </c>
@@ -44558,12 +44791,15 @@
       <c r="G57" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H57" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC9910', TO_DATE('10/6/1999', 'MM/DD/YYYY'), TO_DATE('11/4/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9910'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H57" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I57" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC9910', TO_DATE('10/6/1999', 'MM/DD/YYYY'), TO_DATE('11/4/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9910'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>79</v>
       </c>
@@ -44585,12 +44821,15 @@
       <c r="G58" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H58" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('TC0005', TO_DATE('5/8/2000', 'MM/DD/YYYY'), TO_DATE('5/17/2000', 'MM/DD/YYYY'), 'Leg dates were made up for testing purposes based on the dates in the cast files', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0005'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H58" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I58" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0005', TO_DATE('5/8/2000', 'MM/DD/YYYY'), TO_DATE('5/17/2000', 'MM/DD/YYYY'), 'Leg dates were made up for testing purposes based on the dates in the cast files', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0005'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>341</v>
       </c>
@@ -44612,12 +44851,15 @@
       <c r="G59" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H59" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('RL-17-05 Leg 1', TO_DATE('8/17/2017', 'MM/DD/YYYY'), TO_DATE('9/5/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H59" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I59" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('RL-17-05 Leg 1', TO_DATE('8/17/2017', 'MM/DD/YYYY'), TO_DATE('9/5/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>341</v>
       </c>
@@ -44639,12 +44881,15 @@
       <c r="G60" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H60" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('RL-17-05 Leg 2', TO_DATE('9/11/2017', 'MM/DD/YYYY'), TO_DATE('9/30/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H60" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I60" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('RL-17-05 Leg 2', TO_DATE('9/11/2017', 'MM/DD/YYYY'), TO_DATE('9/30/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>341</v>
       </c>
@@ -44666,12 +44911,15 @@
       <c r="G61" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H61" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('RL-17-05 Leg 3', TO_DATE('10/1/2017', 'MM/DD/YYYY'), TO_DATE('10/10/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H61" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I61" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('RL-17-05 Leg 3', TO_DATE('10/1/2017', 'MM/DD/YYYY'), TO_DATE('10/10/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>341</v>
       </c>
@@ -44693,12 +44941,15 @@
       <c r="G62" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H62" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('RL-17-05 Leg 4', TO_DATE('10/16/2017', 'MM/DD/YYYY'), TO_DATE('11/9/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H62" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I62" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('RL-17-05 Leg 4', TO_DATE('10/16/2017', 'MM/DD/YYYY'), TO_DATE('11/9/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>341</v>
       </c>
@@ -44720,12 +44971,15 @@
       <c r="G63" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H63" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('RL-17-05 Leg 5', TO_DATE('11/15/2017', 'MM/DD/YYYY'), TO_DATE('12/9/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H63" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I63" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('RL-17-05 Leg 5', TO_DATE('11/15/2017', 'MM/DD/YYYY'), TO_DATE('12/9/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>33</v>
       </c>
@@ -44747,12 +45001,15 @@
       <c r="G64" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H64" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-17-06 Leg 1', TO_DATE('7/6/2017', 'MM/DD/YYYY'), TO_DATE('8/2/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H64" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I64" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-17-06 Leg 1', TO_DATE('7/6/2017', 'MM/DD/YYYY'), TO_DATE('8/2/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>33</v>
       </c>
@@ -44774,12 +45031,15 @@
       <c r="G65" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H65" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-17-06 Leg 2', TO_DATE('8/8/2017', 'MM/DD/YYYY'), TO_DATE('9/5/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H65" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I65" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-17-06 Leg 2', TO_DATE('8/8/2017', 'MM/DD/YYYY'), TO_DATE('9/5/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>33</v>
       </c>
@@ -44801,12 +45061,15 @@
       <c r="G66" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H66" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-17-06 Leg 3', TO_DATE('9/11/2017', 'MM/DD/YYYY'), TO_DATE('10/10/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H66" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I66" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-17-06 Leg 3', TO_DATE('9/11/2017', 'MM/DD/YYYY'), TO_DATE('10/10/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>33</v>
       </c>
@@ -44828,12 +45091,15 @@
       <c r="G67" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H67" s="5" t="str">
-        <f t="shared" ref="H67:H68" si="1">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ") values ('", SUBSTITUTE(B67, "'", "''"), "', TO_DATE('", C67, "', 'MM/DD/YYYY'), TO_DATE('", D67, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E67, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F67, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A67, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G67, "'", "''"), "'));")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-19-01', TO_DATE('4/3/2019', 'MM/DD/YYYY'), TO_DATE('4/12/2019', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H67" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I67" s="5" t="str">
+        <f t="shared" ref="I67:I69" si="1">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B67, "'", "''"), "', TO_DATE('", C67, "', 'MM/DD/YYYY'), TO_DATE('", D67, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E67, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F67, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A67, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G67, "'", "''"), "'), '", H67, "');")</f>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-19-01', TO_DATE('4/3/2019', 'MM/DD/YYYY'), TO_DATE('4/12/2019', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>33</v>
       </c>
@@ -44855,109 +45121,125 @@
       <c r="G68" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H68" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-18-03', TO_DATE('7/8/2018', 'MM/DD/YYYY'), TO_DATE('7/31/2018', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-18-03'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="H68" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I68" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-18-03', TO_DATE('7/8/2018', 'MM/DD/YYYY'), TO_DATE('7/31/2018', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-18-03'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>33</v>
+      </c>
+      <c r="B69" t="s">
+        <v>2018</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>2020</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>2021</v>
+      </c>
+      <c r="E69" t="s">
+        <v>2022</v>
+      </c>
+      <c r="F69" t="s">
+        <v>2018</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>1049</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I69" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-19-06', TO_DATE('9/11/2019', 'MM/DD/YYYY'), TO_DATE('9/29/2019', 'MM/DD/YYYY'), 'Leg dates retrieved from project report', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H70" s="6"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>33</v>
-      </c>
-      <c r="B71" t="s">
-        <v>400</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>414</v>
-      </c>
-      <c r="E71" t="s">
-        <v>415</v>
-      </c>
-      <c r="F71" t="s">
-        <v>400</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>1049</v>
-      </c>
-      <c r="H71" s="5" t="str">
-        <f t="shared" ref="H71:H77" si="2">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ") values ('", SUBSTITUTE(B71, "'", "''"), "', TO_DATE('", C71, "', 'MM/DD/YYYY'), TO_DATE('", D71, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E71, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F71, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A71, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G71, "'", "''"), "'));")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-14-01', TO_DATE('3/18/2014', 'MM/DD/YYYY'), TO_DATE('3/27/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H71" s="6"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>33</v>
       </c>
       <c r="B72" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="E72" t="s">
         <v>415</v>
       </c>
       <c r="F72" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H72" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-14-02', TO_DATE('4/6/2014', 'MM/DD/YYYY'), TO_DATE('4/18/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H72" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I72" s="5" t="str">
+        <f t="shared" ref="I72:I78" si="2">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B72, "'", "''"), "', TO_DATE('", C72, "', 'MM/DD/YYYY'), TO_DATE('", D72, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E72, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F72, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A72, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G72, "'", "''"), "'), '", H72, "');")</f>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-14-01', TO_DATE('3/18/2014', 'MM/DD/YYYY'), TO_DATE('3/27/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>33</v>
       </c>
       <c r="B73" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="E73" t="s">
         <v>415</v>
       </c>
       <c r="F73" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H73" s="5" t="str">
+      <c r="H73" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I73" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-14-04 Leg 1', TO_DATE('6/21/2014', 'MM/DD/YYYY'), TO_DATE('7/1/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-14-02', TO_DATE('4/6/2014', 'MM/DD/YYYY'), TO_DATE('4/18/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>33</v>
       </c>
       <c r="B74" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="E74" t="s">
         <v>415</v>
@@ -44968,217 +45250,241 @@
       <c r="G74" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H74" s="5" t="str">
+      <c r="H74" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I74" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-14-04 Leg 2', TO_DATE('7/8/2014', 'MM/DD/YYYY'), TO_DATE('7/19/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-14-04 Leg 1', TO_DATE('6/21/2014', 'MM/DD/YYYY'), TO_DATE('7/1/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>33</v>
       </c>
       <c r="B75" t="s">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E75" t="s">
         <v>415</v>
       </c>
       <c r="F75" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H75" s="5" t="str">
+      <c r="H75" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I75" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-14-05', TO_DATE('7/25/2014', 'MM/DD/YYYY'), TO_DATE('8/23/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-05'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-14-04 Leg 2', TO_DATE('7/8/2014', 'MM/DD/YYYY'), TO_DATE('7/19/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>33</v>
       </c>
       <c r="B76" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E76" t="s">
         <v>415</v>
       </c>
       <c r="F76" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H76" s="5" t="str">
+      <c r="H76" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I76" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-14-06', TO_DATE('8/31/2014', 'MM/DD/YYYY'), TO_DATE('9/18/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-14-05', TO_DATE('7/25/2014', 'MM/DD/YYYY'), TO_DATE('8/23/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-05'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>33</v>
       </c>
       <c r="B77" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E77" t="s">
         <v>415</v>
       </c>
       <c r="F77" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H77" s="5" t="str">
+      <c r="H77" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I77" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-14-07', TO_DATE('10/2/2014', 'MM/DD/YYYY'), TO_DATE('10/27/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-07'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-14-06', TO_DATE('8/31/2014', 'MM/DD/YYYY'), TO_DATE('9/18/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>33</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B78" t="s">
+        <v>412</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="E78" t="s">
+        <v>415</v>
+      </c>
+      <c r="F78" t="s">
+        <v>412</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>1049</v>
+      </c>
+      <c r="H78" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I78" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-14-07', TO_DATE('10/2/2014', 'MM/DD/YYYY'), TO_DATE('10/27/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-07'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>33</v>
+      </c>
+      <c r="B81" t="s">
         <v>75</v>
       </c>
-      <c r="C80" s="8" t="s">
+      <c r="C81" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="D81" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E81" t="s">
         <v>415</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F81" t="s">
         <v>75</v>
       </c>
-      <c r="G80" s="5" t="s">
+      <c r="G81" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H80" s="5" t="str">
-        <f>CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ") values ('", SUBSTITUTE(B80, "'", "''"), "', TO_DATE('", C80, "', 'MM/DD/YYYY'), TO_DATE('", D80, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E80, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F80, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A80, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G80, "'", "''"), "'));")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-15-01', TO_DATE('4/3/2015', 'MM/DD/YYYY'), TO_DATE('4/14/2015', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-15-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+      <c r="H81" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I81" s="5" t="str">
+        <f>CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B81, "'", "''"), "', TO_DATE('", C81, "', 'MM/DD/YYYY'), TO_DATE('", D81, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E81, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F81, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A81, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G81, "'", "''"), "'), '", H81, "');")</f>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-15-01', TO_DATE('4/3/2015', 'MM/DD/YYYY'), TO_DATE('4/14/2015', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-15-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>1884</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>33</v>
       </c>
-      <c r="B86" s="9" t="s">
+      <c r="B87" s="9" t="s">
         <v>1885</v>
       </c>
-      <c r="C86" s="8" t="s">
+      <c r="C87" s="8" t="s">
         <v>1915</v>
       </c>
-      <c r="D86" s="8" t="s">
+      <c r="D87" s="8" t="s">
         <v>1927</v>
-      </c>
-      <c r="E86" t="s">
-        <v>1904</v>
-      </c>
-      <c r="F86" s="9" t="s">
-        <v>1881</v>
-      </c>
-      <c r="G86" s="5" t="s">
-        <v>1049</v>
-      </c>
-      <c r="H86" s="5" t="str">
-        <f>CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ") values ('", SUBSTITUTE(B86, "'", "''"), "', TO_DATE('", C86, "', 'MM/DD/YYYY'), TO_DATE('", D86, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E86, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F86, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A86, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G86, "'", "''"), "'));")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-20-04 Leg 1', TO_DATE('3/20/2020', 'MM/DD/YYYY'), TO_DATE('4/15/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-20-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B87" s="16" t="s">
-        <v>1903</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>1916</v>
-      </c>
-      <c r="D87" s="8" t="s">
-        <v>1928</v>
       </c>
       <c r="E87" t="s">
         <v>1904</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H87" s="5" t="str">
-        <f>CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ") values ('", SUBSTITUTE(B87, "'", "''"), "', TO_DATE('", C87, "', 'MM/DD/YYYY'), TO_DATE('", D87, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E87, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F87, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A87, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G87, "'", "''"), "'));")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-20-05 Leg 1', TO_DATE('4/10/2020', 'MM/DD/YYYY'), TO_DATE('4/25/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-20-05'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="H87" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I87" s="5" t="str">
+        <f t="shared" ref="I87:I122" si="3">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B87, "'", "''"), "', TO_DATE('", C87, "', 'MM/DD/YYYY'), TO_DATE('", D87, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E87, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F87, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A87, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G87, "'", "''"), "'), '", H87, "');")</f>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-20-04 Leg 1', TO_DATE('3/20/2020', 'MM/DD/YYYY'), TO_DATE('4/15/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-20-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B88" t="s">
-        <v>1887</v>
+      <c r="B88" s="16" t="s">
+        <v>1903</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>1905</v>
+        <v>1916</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>1917</v>
+        <v>1928</v>
       </c>
       <c r="E88" t="s">
-        <v>1929</v>
+        <v>1904</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>1896</v>
+        <v>1882</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H88" s="5" t="str">
-        <f t="shared" ref="H88:H92" si="3">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ") values ('", SUBSTITUTE(B88, "'", "''"), "', TO_DATE('", C88, "', 'MM/DD/YYYY'), TO_DATE('", D88, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E88, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F88, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A88, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G88, "'", "''"), "'));")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-21-01 Leg 1', TO_DATE('10/15/2020', 'MM/DD/YYYY'), TO_DATE('10/30/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H88" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I88" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-20-05 Leg 1', TO_DATE('4/10/2020', 'MM/DD/YYYY'), TO_DATE('4/25/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-20-05'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>33</v>
       </c>
       <c r="B89" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="E89" t="s">
         <v>1929</v>
@@ -45189,77 +45495,86 @@
       <c r="G89" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H89" s="5" t="str">
+      <c r="H89" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I89" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-21-01 Leg 2', TO_DATE('11/5/2020', 'MM/DD/YYYY'), TO_DATE('11/20/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="16" t="s">
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-01 Leg 1', TO_DATE('10/15/2020', 'MM/DD/YYYY'), TO_DATE('10/30/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>33</v>
       </c>
-      <c r="B90" s="16" t="s">
-        <v>1889</v>
+      <c r="B90" t="s">
+        <v>1888</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="E90" t="s">
         <v>1929</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>1889</v>
+        <v>1896</v>
       </c>
       <c r="G90" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H90" s="5" t="str">
+      <c r="H90" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I90" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-21-03', TO_DATE('11/15/2020', 'MM/DD/YYYY'), TO_DATE('12/1/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-03'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-01 Leg 2', TO_DATE('11/5/2020', 'MM/DD/YYYY'), TO_DATE('11/20/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B91" t="s">
-        <v>1890</v>
+      <c r="B91" s="16" t="s">
+        <v>1889</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="E91" t="s">
         <v>1929</v>
       </c>
       <c r="F91" s="9" t="s">
-        <v>1897</v>
+        <v>1889</v>
       </c>
       <c r="G91" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H91" s="5" t="str">
+      <c r="H91" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I91" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-21-04 Leg 1', TO_DATE('11/22/2020', 'MM/DD/YYYY'), TO_DATE('11/28/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-03', TO_DATE('11/15/2020', 'MM/DD/YYYY'), TO_DATE('12/1/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-03'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>33</v>
       </c>
       <c r="B92" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="E92" t="s">
         <v>1929</v>
@@ -45270,77 +45585,86 @@
       <c r="G92" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H92" s="5" t="str">
+      <c r="H92" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I92" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-21-04 Leg 2', TO_DATE('11/30/2020', 'MM/DD/YYYY'), TO_DATE('12/10/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-04 Leg 1', TO_DATE('11/22/2020', 'MM/DD/YYYY'), TO_DATE('11/28/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>4</v>
-      </c>
-      <c r="B93" s="9" t="s">
-        <v>1892</v>
+        <v>33</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1891</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="E93" t="s">
-        <v>1899</v>
+        <v>1929</v>
       </c>
       <c r="F93" s="9" t="s">
-        <v>1892</v>
+        <v>1897</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H93" s="5" t="str">
-        <f t="shared" ref="H93:H97" si="4">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ") values ('", SUBSTITUTE(B93, "'", "''"), "', TO_DATE('", C93, "', 'MM/DD/YYYY'), TO_DATE('", D93, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E93, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F93, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A93, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G93, "'", "''"), "'));")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI-21-06', TO_DATE('3/15/2021', 'MM/DD/YYYY'), TO_DATE('3/30/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-06'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H93" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I93" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-04 Leg 2', TO_DATE('11/30/2020', 'MM/DD/YYYY'), TO_DATE('12/10/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>4</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="E94" t="s">
         <v>1899</v>
       </c>
       <c r="F94" s="9" t="s">
-        <v>1898</v>
+        <v>1892</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H94" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI-21-07 Leg 1', TO_DATE('3/27/2021', 'MM/DD/YYYY'), TO_DATE('4/15/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-07'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H94" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I94" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-21-06', TO_DATE('3/15/2021', 'MM/DD/YYYY'), TO_DATE('3/30/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-06'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>4</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="E95" t="s">
         <v>1899</v>
@@ -45351,50 +45675,56 @@
       <c r="G95" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H95" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI-21-07 Leg 2', TO_DATE('4/18/2021', 'MM/DD/YYYY'), TO_DATE('4/30/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-07'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="16" t="s">
+      <c r="H95" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I95" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-21-07 Leg 1', TO_DATE('3/27/2021', 'MM/DD/YYYY'), TO_DATE('4/15/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-07'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>4</v>
       </c>
-      <c r="B96" s="16" t="s">
-        <v>1900</v>
+      <c r="B96" s="9" t="s">
+        <v>1894</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="E96" t="s">
         <v>1899</v>
       </c>
       <c r="F96" s="9" t="s">
-        <v>1895</v>
+        <v>1898</v>
       </c>
       <c r="G96" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H96" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI-21-08 Leg 1', TO_DATE('4/28/2021', 'MM/DD/YYYY'), TO_DATE('5/23/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="H96" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I96" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-21-07 Leg 2', TO_DATE('4/18/2021', 'MM/DD/YYYY'), TO_DATE('4/30/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-07'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B97" s="9" t="s">
-        <v>1901</v>
+      <c r="B97" s="16" t="s">
+        <v>1900</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="E97" t="s">
         <v>1899</v>
@@ -45405,50 +45735,56 @@
       <c r="G97" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H97" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI-21-08 Leg 2', TO_DATE('5/25/2021', 'MM/DD/YYYY'), TO_DATE('6/17/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H97" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I97" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-21-08 Leg 1', TO_DATE('4/28/2021', 'MM/DD/YYYY'), TO_DATE('5/23/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>4</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>1930</v>
+        <v>1901</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>1935</v>
+        <v>1914</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>1936</v>
+        <v>1926</v>
       </c>
       <c r="E98" t="s">
-        <v>1902</v>
+        <v>1899</v>
       </c>
       <c r="F98" s="9" t="s">
-        <v>1886</v>
+        <v>1895</v>
       </c>
       <c r="G98" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H98" s="5" t="str">
-        <f t="shared" ref="H98:H102" si="5">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ") values ('", SUBSTITUTE(B98, "'", "''"), "', TO_DATE('", C98, "', 'MM/DD/YYYY'), TO_DATE('", D98, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E98, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F98, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A98, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G98, "'", "''"), "'));")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI-20-08 Leg 1', TO_DATE('6/10/2020', 'MM/DD/YYYY'), TO_DATE('6/29/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H98" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I98" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-21-08 Leg 2', TO_DATE('5/25/2021', 'MM/DD/YYYY'), TO_DATE('6/17/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>4</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>1937</v>
+        <v>1935</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>1938</v>
+        <v>1936</v>
       </c>
       <c r="E99" t="s">
         <v>1902</v>
@@ -45459,50 +45795,56 @@
       <c r="G99" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H99" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI-20-08 Leg 2', TO_DATE('7/2/2020', 'MM/DD/YYYY'), TO_DATE('7/26/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H99" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I99" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-20-08 Leg 1', TO_DATE('6/10/2020', 'MM/DD/YYYY'), TO_DATE('6/29/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>4</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>1940</v>
+        <v>1938</v>
       </c>
       <c r="E100" t="s">
         <v>1902</v>
       </c>
       <c r="F100" s="9" t="s">
-        <v>1945</v>
+        <v>1886</v>
       </c>
       <c r="G100" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H100" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI-20-09 Leg 1', TO_DATE('7/20/2020', 'MM/DD/YYYY'), TO_DATE('8/12/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-09'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H100" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I100" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-20-08 Leg 2', TO_DATE('7/2/2020', 'MM/DD/YYYY'), TO_DATE('7/26/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>4</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>1941</v>
+        <v>1939</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
       <c r="E101" t="s">
         <v>1902</v>
@@ -45513,77 +45855,86 @@
       <c r="G101" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H101" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI-20-09 Leg 2', TO_DATE('8/16/2020', 'MM/DD/YYYY'), TO_DATE('9/2/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-09'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="16" t="s">
+      <c r="H101" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I101" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-20-09 Leg 1', TO_DATE('7/20/2020', 'MM/DD/YYYY'), TO_DATE('8/12/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-09'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>4</v>
       </c>
-      <c r="B102" s="16" t="s">
-        <v>1934</v>
+      <c r="B102" s="9" t="s">
+        <v>1933</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>1944</v>
+        <v>1941</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="E102" t="s">
         <v>1902</v>
       </c>
       <c r="F102" s="9" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="G102" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H102" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI-20-10 Leg 1', TO_DATE('6/14/2020', 'MM/DD/YYYY'), TO_DATE('7/30/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-10'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>33</v>
-      </c>
-      <c r="B103" s="9" t="s">
-        <v>1948</v>
+      <c r="H102" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I102" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-20-09 Leg 2', TO_DATE('8/16/2020', 'MM/DD/YYYY'), TO_DATE('9/2/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-09'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103" s="16" t="s">
+        <v>1934</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>1958</v>
+        <v>1944</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>1959</v>
+        <v>1943</v>
       </c>
       <c r="E103" t="s">
-        <v>1953</v>
+        <v>1902</v>
       </c>
       <c r="F103" s="9" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="G103" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H103" s="5" t="str">
-        <f t="shared" ref="H103:H107" si="6">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ") values ('", SUBSTITUTE(B103, "'", "''"), "', TO_DATE('", C103, "', 'MM/DD/YYYY'), TO_DATE('", D103, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E103, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F103, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A103, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G103, "'", "''"), "'));")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-21-06 Leg 1', TO_DATE('1/12/2021', 'MM/DD/YYYY'), TO_DATE('1/31/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H103" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I103" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-20-10 Leg 1', TO_DATE('6/14/2020', 'MM/DD/YYYY'), TO_DATE('7/30/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-10'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>33</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>1961</v>
+        <v>1959</v>
       </c>
       <c r="E104" t="s">
         <v>1953</v>
@@ -45594,77 +45945,86 @@
       <c r="G104" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H104" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-21-06 Leg 2', TO_DATE('2/3/2021', 'MM/DD/YYYY'), TO_DATE('2/25/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="18" t="s">
+      <c r="H104" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I104" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-06 Leg 1', TO_DATE('1/12/2021', 'MM/DD/YYYY'), TO_DATE('1/31/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>33</v>
       </c>
-      <c r="B105" s="18" t="s">
-        <v>1950</v>
+      <c r="B105" s="9" t="s">
+        <v>1949</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>1966</v>
+        <v>1960</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>1967</v>
+        <v>1961</v>
       </c>
       <c r="E105" t="s">
         <v>1953</v>
       </c>
       <c r="F105" s="9" t="s">
-        <v>1950</v>
+        <v>1947</v>
       </c>
       <c r="G105" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H105" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-21-07', TO_DATE('1/30/2021', 'MM/DD/YYYY'), TO_DATE('3/6/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-07'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="H105" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I105" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-06 Leg 2', TO_DATE('2/3/2021', 'MM/DD/YYYY'), TO_DATE('2/25/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B106" s="9" t="s">
-        <v>1951</v>
+      <c r="B106" s="18" t="s">
+        <v>1950</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>1962</v>
+        <v>1966</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>1963</v>
+        <v>1967</v>
       </c>
       <c r="E106" t="s">
         <v>1953</v>
       </c>
       <c r="F106" s="9" t="s">
-        <v>1954</v>
+        <v>1950</v>
       </c>
       <c r="G106" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H106" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-21-08 Leg 1', TO_DATE('3/2/2021', 'MM/DD/YYYY'), TO_DATE('3/23/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-08'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H106" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I106" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-07', TO_DATE('1/30/2021', 'MM/DD/YYYY'), TO_DATE('3/6/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-07'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>33</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>1964</v>
+        <v>1962</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>1965</v>
+        <v>1963</v>
       </c>
       <c r="E107" t="s">
         <v>1953</v>
@@ -45675,50 +46035,56 @@
       <c r="G107" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H107" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-21-08 Leg 2', TO_DATE('3/26/2021', 'MM/DD/YYYY'), TO_DATE('4/12/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-08'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H107" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I107" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-08 Leg 1', TO_DATE('3/2/2021', 'MM/DD/YYYY'), TO_DATE('3/23/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-08'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>33</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>1955</v>
+        <v>1952</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>1968</v>
+        <v>1964</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>1969</v>
+        <v>1965</v>
       </c>
       <c r="E108" t="s">
         <v>1953</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>1956</v>
+        <v>1954</v>
       </c>
       <c r="G108" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H108" s="5" t="str">
-        <f t="shared" ref="H108" si="7">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ") values ('", SUBSTITUTE(B108, "'", "''"), "', TO_DATE('", C108, "', 'MM/DD/YYYY'), TO_DATE('", D108, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E108, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F108, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A108, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G108, "'", "''"), "'));")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-21-09 Leg 1', TO_DATE('5/11/2021', 'MM/DD/YYYY'), TO_DATE('5/30/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-09'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H108" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I108" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-08 Leg 2', TO_DATE('3/26/2021', 'MM/DD/YYYY'), TO_DATE('4/12/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-08'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>33</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>1970</v>
+        <v>1968</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>1971</v>
+        <v>1969</v>
       </c>
       <c r="E109" t="s">
         <v>1953</v>
@@ -45729,50 +46095,56 @@
       <c r="G109" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H109" s="5" t="str">
-        <f t="shared" ref="H109" si="8">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ") values ('", SUBSTITUTE(B109, "'", "''"), "', TO_DATE('", C109, "', 'MM/DD/YYYY'), TO_DATE('", D109, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E109, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F109, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A109, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G109, "'", "''"), "'));")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-21-09 Leg 2', TO_DATE('6/2/2021', 'MM/DD/YYYY'), TO_DATE('6/19/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-09'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H109" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I109" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-09 Leg 1', TO_DATE('5/11/2021', 'MM/DD/YYYY'), TO_DATE('5/30/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-09'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>1988</v>
+        <v>1957</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>1992</v>
+        <v>1970</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>1993</v>
+        <v>1971</v>
       </c>
       <c r="E110" t="s">
-        <v>1985</v>
+        <v>1953</v>
       </c>
       <c r="F110" s="9" t="s">
-        <v>2000</v>
+        <v>1956</v>
       </c>
       <c r="G110" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H110" s="5" t="str">
-        <f t="shared" ref="H110:H113" si="9">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ") values ('", SUBSTITUTE(B110, "'", "''"), "', TO_DATE('", C110, "', 'MM/DD/YYYY'), TO_DATE('", D110, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E110, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F110, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A110, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G110, "'", "''"), "'));")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-19-04 Leg 1', TO_DATE('6/1/2019', 'MM/DD/YYYY'), TO_DATE('6/15/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-04'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H110" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I110" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-09 Leg 2', TO_DATE('6/2/2021', 'MM/DD/YYYY'), TO_DATE('6/19/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-09'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>4</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="E111" t="s">
         <v>1985</v>
@@ -45783,50 +46155,56 @@
       <c r="G111" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H111" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-19-04 Leg 2', TO_DATE('6/19/2019', 'MM/DD/YYYY'), TO_DATE('7/12/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-04'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="17" t="s">
+      <c r="H111" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I111" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-19-04 Leg 1', TO_DATE('6/1/2019', 'MM/DD/YYYY'), TO_DATE('6/15/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-04'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>4</v>
       </c>
-      <c r="B112" s="17" t="s">
-        <v>1990</v>
+      <c r="B112" s="9" t="s">
+        <v>1989</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="E112" t="s">
         <v>1985</v>
       </c>
       <c r="F112" s="9" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G112" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H112" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-19-05 Leg 1', TO_DATE('7/14/2019', 'MM/DD/YYYY'), TO_DATE('7/31/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-05'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="H112" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I112" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-19-04 Leg 2', TO_DATE('6/19/2019', 'MM/DD/YYYY'), TO_DATE('7/12/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-04'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B113" s="9" t="s">
-        <v>1991</v>
+      <c r="B113" s="17" t="s">
+        <v>1990</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="E113" t="s">
         <v>1985</v>
@@ -45837,50 +46215,56 @@
       <c r="G113" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H113" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-19-05 Leg 2', TO_DATE('8/2/2019', 'MM/DD/YYYY'), TO_DATE('8/15/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-05'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H113" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I113" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-19-05 Leg 1', TO_DATE('7/14/2019', 'MM/DD/YYYY'), TO_DATE('7/31/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-05'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>4</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>1973</v>
+        <v>1991</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>1976</v>
+        <v>1998</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>1977</v>
+        <v>1999</v>
       </c>
       <c r="E114" t="s">
-        <v>1987</v>
+        <v>1985</v>
       </c>
       <c r="F114" s="9" t="s">
-        <v>1972</v>
+        <v>2001</v>
       </c>
       <c r="G114" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H114" s="5" t="str">
-        <f t="shared" ref="H114:H117" si="10">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ") values ('", SUBSTITUTE(B114, "'", "''"), "', TO_DATE('", C114, "', 'MM/DD/YYYY'), TO_DATE('", D114, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E114, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F114, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A114, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G114, "'", "''"), "'));")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI-19-01 Leg 1', TO_DATE('10/15/2018', 'MM/DD/YYYY'), TO_DATE('11/2/2018', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-19-01'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H114" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I114" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-19-05 Leg 2', TO_DATE('8/2/2019', 'MM/DD/YYYY'), TO_DATE('8/15/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-05'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>4</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>1984</v>
+        <v>1973</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>1978</v>
+        <v>1976</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>1979</v>
+        <v>1977</v>
       </c>
       <c r="E115" t="s">
         <v>1987</v>
@@ -45891,50 +46275,56 @@
       <c r="G115" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H115" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI-19-01 Leg 2', TO_DATE('11/5/2018', 'MM/DD/YYYY'), TO_DATE('11/29/2018', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-19-01'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="18" t="s">
+      <c r="H115" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I115" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-19-01 Leg 1', TO_DATE('10/15/2018', 'MM/DD/YYYY'), TO_DATE('11/2/2018', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-19-01'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>4</v>
       </c>
-      <c r="B116" s="18" t="s">
-        <v>1974</v>
+      <c r="B116" s="9" t="s">
+        <v>1984</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>1980</v>
+        <v>1978</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>1981</v>
+        <v>1979</v>
       </c>
       <c r="E116" t="s">
         <v>1987</v>
       </c>
       <c r="F116" s="9" t="s">
-        <v>1986</v>
+        <v>1972</v>
       </c>
       <c r="G116" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H116" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI-19-02 Leg 1', TO_DATE('11/20/2018', 'MM/DD/YYYY'), TO_DATE('12/10/2018', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-19-02'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="H116" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I116" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-19-01 Leg 2', TO_DATE('11/5/2018', 'MM/DD/YYYY'), TO_DATE('11/29/2018', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-19-01'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B117" s="9" t="s">
-        <v>1975</v>
+      <c r="B117" s="18" t="s">
+        <v>1974</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>1982</v>
+        <v>1980</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>1983</v>
+        <v>1981</v>
       </c>
       <c r="E117" t="s">
         <v>1987</v>
@@ -45945,50 +46335,56 @@
       <c r="G117" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H117" s="5" t="str">
-        <f t="shared" si="10"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('HI-19-02 Leg 2', TO_DATE('12/12/2018', 'MM/DD/YYYY'), TO_DATE('12/30/2018', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-19-02'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H117" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I117" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-19-02 Leg 1', TO_DATE('11/20/2018', 'MM/DD/YYYY'), TO_DATE('12/10/2018', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-19-02'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>2015</v>
+        <v>1975</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>2006</v>
+        <v>1982</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>2007</v>
+        <v>1983</v>
       </c>
       <c r="E118" t="s">
-        <v>2002</v>
+        <v>1987</v>
       </c>
       <c r="F118" s="9" t="s">
-        <v>2014</v>
+        <v>1986</v>
       </c>
       <c r="G118" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H118" s="5" t="str">
-        <f t="shared" ref="H118:H121" si="11">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ") values ('", SUBSTITUTE(B118, "'", "''"), "', TO_DATE('", C118, "', 'MM/DD/YYYY'), TO_DATE('", D118, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E118, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F118, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A118, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G118, "'", "''"), "'));")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-22-01 Leg 1', TO_DATE('10/21/2021', 'MM/DD/YYYY'), TO_DATE('11/13/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H118" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I118" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-19-02 Leg 2', TO_DATE('12/12/2018', 'MM/DD/YYYY'), TO_DATE('12/30/2018', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-19-02'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>33</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="E119" t="s">
         <v>2002</v>
@@ -45999,50 +46395,56 @@
       <c r="G119" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H119" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-22-01 Leg 2', TO_DATE('11/15/2021', 'MM/DD/YYYY'), TO_DATE('12/4/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="16" t="s">
+      <c r="H119" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I119" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-22-01 Leg 1', TO_DATE('10/21/2021', 'MM/DD/YYYY'), TO_DATE('11/13/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>33</v>
       </c>
-      <c r="B120" s="16" t="s">
-        <v>2004</v>
+      <c r="B120" s="9" t="s">
+        <v>2016</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="E120" t="s">
         <v>2002</v>
       </c>
       <c r="F120" s="9" t="s">
-        <v>2005</v>
+        <v>2014</v>
       </c>
       <c r="G120" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H120" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-22-02 Leg 1', TO_DATE('11/30/2021', 'MM/DD/YYYY'), TO_DATE('12/15/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="H120" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I120" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-22-01 Leg 2', TO_DATE('11/15/2021', 'MM/DD/YYYY'), TO_DATE('12/4/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B121" s="9" t="s">
-        <v>2003</v>
+      <c r="B121" s="16" t="s">
+        <v>2004</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="E121" t="s">
         <v>2002</v>
@@ -46053,9 +46455,42 @@
       <c r="G121" s="5" t="s">
         <v>1049</v>
       </c>
-      <c r="H121" s="5" t="str">
-        <f t="shared" si="11"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID) values ('SE-22-02 Leg 2', TO_DATE('12/17/2021', 'MM/DD/YYYY'), TO_DATE('1/12/2022', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'));</v>
+      <c r="H121" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I121" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-22-02 Leg 1', TO_DATE('11/30/2021', 'MM/DD/YYYY'), TO_DATE('12/15/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>33</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>2003</v>
+      </c>
+      <c r="C122" s="8" t="s">
+        <v>2012</v>
+      </c>
+      <c r="D122" s="8" t="s">
+        <v>2013</v>
+      </c>
+      <c r="E122" t="s">
+        <v>2002</v>
+      </c>
+      <c r="F122" s="9" t="s">
+        <v>2005</v>
+      </c>
+      <c r="G122" s="5" t="s">
+        <v>1049</v>
+      </c>
+      <c r="H122" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I122" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-22-02 Leg 2', TO_DATE('12/17/2021', 'MM/DD/YYYY'), TO_DATE('1/12/2022', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
       </c>
     </row>
   </sheetData>
@@ -49024,7 +49459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D44" sqref="D43:D44"/>
     </sheetView>
   </sheetViews>
@@ -50043,9 +50478,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C155"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43:C45"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C137" sqref="C137:C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51684,6 +52119,30 @@
       <c r="C136" s="5" t="str">
         <f t="shared" si="1"/>
         <v>insert into ccd_leg_aliases (cruise_leg_id, LEG_ALIAS_NAME) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = 'SE-18-03'), 'SE1803');</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>2018</v>
+      </c>
+      <c r="B137" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C137" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into ccd_leg_aliases (cruise_leg_id, LEG_ALIAS_NAME) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = 'SE-19-06'), 'SE1906');</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>2018</v>
+      </c>
+      <c r="B138" t="s">
+        <v>2018</v>
+      </c>
+      <c r="C138" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into ccd_leg_aliases (cruise_leg_id, LEG_ALIAS_NAME) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = 'SE-19-06'), 'SE-19-06');</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated the DB/APEX app to rename the cruise leg timezone name updated the load_ref_data.sql and Cruise_Leg_DDL_DML_generator.xlsx to include the new timezone field
</commit_message>
<xml_diff>
--- a/docs/Cruise_Leg_DDL_DML_generator.xlsx
+++ b/docs/Cruise_Leg_DDL_DML_generator.xlsx
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4953" uniqueCount="2026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4953" uniqueCount="2027">
   <si>
     <t>Cruise Name</t>
   </si>
@@ -6212,10 +6212,13 @@
     <t>SE1906</t>
   </si>
   <si>
-    <t>UTC_TZ_OFFSET</t>
-  </si>
-  <si>
     <t>-10:00</t>
+  </si>
+  <si>
+    <t>TZ_NAME</t>
+  </si>
+  <si>
+    <t>US/Hawaii</t>
   </si>
 </sst>
 </file>
@@ -43246,8 +43249,8 @@
   <dimension ref="A1:I122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I69" sqref="I2:I69"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H87" sqref="H87:H122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43281,7 +43284,7 @@
         <v>1725</v>
       </c>
       <c r="H1" t="s">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="I1" t="s">
         <v>109</v>
@@ -43307,11 +43310,11 @@
         <v>1049</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I2" s="5" t="str">
         <f>CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B2, "'", "''"), "', TO_DATE('", C2, "', 'MM/DD/YYYY'), TO_DATE('", D2, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E2, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F2, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A2, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G2, "'", "''"), "'), '", H2, "');")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-17-07', TO_DATE('10/20/2017', 'MM/DD/YYYY'), TO_DATE('11/03/2017', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-07'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-17-07', TO_DATE('10/20/2017', 'MM/DD/YYYY'), TO_DATE('11/03/2017', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-07'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43334,11 +43337,11 @@
         <v>1049</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="I3" s="5" t="str">
         <f t="shared" ref="I3:I66" si="0">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B3, "'", "''"), "', TO_DATE('", C3, "', 'MM/DD/YYYY'), TO_DATE('", D3, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E3, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F3, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A3, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G3, "'", "''"), "'), '", H3, "');")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-18-06', TO_DATE('10/17/2018', 'MM/DD/YYYY'), TO_DATE('10/31/2018', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-18-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-18-06', TO_DATE('10/17/2018', 'MM/DD/YYYY'), TO_DATE('10/31/2018', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-18-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43361,11 +43364,11 @@
         <v>1049</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="I4" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-17-02', TO_DATE('3/1/2017', 'MM/DD/YYYY'), TO_DATE('3/15/2017', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-17-02', TO_DATE('3/1/2017', 'MM/DD/YYYY'), TO_DATE('3/15/2017', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43388,11 +43391,11 @@
         <v>1049</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="I5" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-15-01', TO_DATE('4/3/2015', 'MM/DD/YYYY'), TO_DATE('4/14/2015', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-15-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-15-01', TO_DATE('4/3/2015', 'MM/DD/YYYY'), TO_DATE('4/14/2015', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-15-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43415,11 +43418,11 @@
         <v>1049</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I6" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HA1201_LEG_I', TO_DATE('2/27/2012', 'MM/DD/YYYY'), TO_DATE('3/25/2012', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1201'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HA1201_LEG_I', TO_DATE('2/27/2012', 'MM/DD/YYYY'), TO_DATE('3/25/2012', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1201'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43442,11 +43445,11 @@
         <v>1049</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I7" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HA1201_LEG_II&amp;III', TO_DATE('4/1/2012', 'MM/DD/YYYY'), TO_DATE('4/27/2012', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1201'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HA1201_LEG_II&amp;III', TO_DATE('4/1/2012', 'MM/DD/YYYY'), TO_DATE('4/27/2012', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1201'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43469,11 +43472,11 @@
         <v>1049</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I8" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HA1201_LEG_IV', TO_DATE('4/27/2012', 'MM/DD/YYYY'), TO_DATE('5/24/2012', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1201'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HA1201_LEG_IV', TO_DATE('4/27/2012', 'MM/DD/YYYY'), TO_DATE('5/24/2012', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1201'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43496,11 +43499,11 @@
         <v>1049</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I9" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HA1101_LEG_I', TO_DATE('3/10/2011', 'MM/DD/YYYY'), TO_DATE('4/5/2011', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1101'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HA1101_LEG_I', TO_DATE('3/10/2011', 'MM/DD/YYYY'), TO_DATE('4/5/2011', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1101'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43523,11 +43526,11 @@
         <v>1049</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I10" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HA1101_LEG_II', TO_DATE('4/7/2011', 'MM/DD/YYYY'), TO_DATE('5/9/2011', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1101'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HA1101_LEG_II', TO_DATE('4/7/2011', 'MM/DD/YYYY'), TO_DATE('5/9/2011', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1101'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43550,11 +43553,11 @@
         <v>1049</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I11" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HA1101_LEG_III', TO_DATE('5/12/2011', 'MM/DD/YYYY'), TO_DATE('5/24/2011', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1101'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HA1101_LEG_III', TO_DATE('5/12/2011', 'MM/DD/YYYY'), TO_DATE('5/24/2011', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1101'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43577,11 +43580,11 @@
         <v>1049</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I12" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HA1007', TO_DATE('9/4/2010', 'MM/DD/YYYY'), TO_DATE('9/29/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1007'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HA1007', TO_DATE('9/4/2010', 'MM/DD/YYYY'), TO_DATE('9/29/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1007'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43604,11 +43607,11 @@
         <v>1049</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I13" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HA1008', TO_DATE('10/7/2010', 'MM/DD/YYYY'), TO_DATE('11/5/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1008'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HA1008', TO_DATE('10/7/2010', 'MM/DD/YYYY'), TO_DATE('11/5/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HA1008'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43631,11 +43634,11 @@
         <v>1049</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I14" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI0401', TO_DATE('9/13/2004', 'MM/DD/YYYY'), TO_DATE('10/17/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0401'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI0401', TO_DATE('9/13/2004', 'MM/DD/YYYY'), TO_DATE('10/17/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0401'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43658,11 +43661,11 @@
         <v>1049</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I15" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI0602', TO_DATE('2/9/2006', 'MM/DD/YYYY'), TO_DATE('3/10/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0602'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI0602', TO_DATE('2/9/2006', 'MM/DD/YYYY'), TO_DATE('3/10/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0602'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43685,11 +43688,11 @@
         <v>1049</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I16" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI0604', TO_DATE('3/15/2006', 'MM/DD/YYYY'), TO_DATE('4/8/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0604'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI0604', TO_DATE('3/15/2006', 'MM/DD/YYYY'), TO_DATE('4/8/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0604'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43712,11 +43715,11 @@
         <v>1049</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I17" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI0609', TO_DATE('6/23/2006', 'MM/DD/YYYY'), TO_DATE('7/20/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0609'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI0609', TO_DATE('6/23/2006', 'MM/DD/YYYY'), TO_DATE('7/20/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0609'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43739,11 +43742,11 @@
         <v>1049</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I18" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI0610', TO_DATE('7/27/2006', 'MM/DD/YYYY'), TO_DATE('8/20/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0610'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI0610', TO_DATE('7/27/2006', 'MM/DD/YYYY'), TO_DATE('8/20/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0610'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43766,11 +43769,11 @@
         <v>1049</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I19" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI0611', TO_DATE('9/1/2006', 'MM/DD/YYYY'), TO_DATE('10/4/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0611'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI0611', TO_DATE('9/1/2006', 'MM/DD/YYYY'), TO_DATE('10/4/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0611'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43793,11 +43796,11 @@
         <v>1049</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I20" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI0701', TO_DATE('4/19/2007', 'MM/DD/YYYY'), TO_DATE('5/9/2007', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0701'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI0701', TO_DATE('4/19/2007', 'MM/DD/YYYY'), TO_DATE('5/9/2007', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI0701'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43820,11 +43823,11 @@
         <v>1049</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I21" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI1001_LEGI', TO_DATE('1/21/2010', 'MM/DD/YYYY'), TO_DATE('2/14/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1001'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI1001_LEGI', TO_DATE('1/21/2010', 'MM/DD/YYYY'), TO_DATE('2/14/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1001'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43847,11 +43850,11 @@
         <v>1049</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I22" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI1001_LEGII', TO_DATE('2/17/2010', 'MM/DD/YYYY'), TO_DATE('3/23/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1001'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI1001_LEGII', TO_DATE('2/17/2010', 'MM/DD/YYYY'), TO_DATE('3/23/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1001'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43874,11 +43877,11 @@
         <v>1049</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="I23" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI1001_LEGIII', TO_DATE('3/27/2010', 'MM/DD/YYYY'), TO_DATE('4/24/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1001'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI1001_LEGIII', TO_DATE('3/27/2010', 'MM/DD/YYYY'), TO_DATE('4/24/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1001'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43901,11 +43904,11 @@
         <v>1049</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="I24" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0304', TO_DATE('5/13/2003', 'MM/DD/YYYY'), TO_DATE('5/28/2003', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0304'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0304', TO_DATE('5/13/2003', 'MM/DD/YYYY'), TO_DATE('5/28/2003', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0304'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43928,11 +43931,11 @@
         <v>1049</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="I25" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0306', TO_DATE('7/12/2003', 'MM/DD/YYYY'), TO_DATE('8/17/2003', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0306'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0306', TO_DATE('7/12/2003', 'MM/DD/YYYY'), TO_DATE('8/17/2003', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0306'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43955,11 +43958,11 @@
         <v>1049</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="I26" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0407', TO_DATE('5/30/2004', 'MM/DD/YYYY'), TO_DATE('6/14/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0407'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0407', TO_DATE('5/30/2004', 'MM/DD/YYYY'), TO_DATE('6/14/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0407'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43982,11 +43985,11 @@
         <v>1049</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="I27" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0410', TO_DATE('7/30/2004', 'MM/DD/YYYY'), TO_DATE('8/16/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0410'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0410', TO_DATE('7/30/2004', 'MM/DD/YYYY'), TO_DATE('8/16/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0410'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44009,11 +44012,11 @@
         <v>1049</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="I28" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0411_LEGI', TO_DATE('8/7/2004', 'MM/DD/YYYY'), TO_DATE('9/7/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0411'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0411_LEGI', TO_DATE('8/7/2004', 'MM/DD/YYYY'), TO_DATE('9/7/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0411'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44036,11 +44039,11 @@
         <v>1049</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="I29" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0411_LEGII', TO_DATE('9/8/2004', 'MM/DD/YYYY'), TO_DATE('9/13/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0411'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0411_LEGII', TO_DATE('9/8/2004', 'MM/DD/YYYY'), TO_DATE('9/13/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0411'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44063,11 +44066,11 @@
         <v>1049</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="I30" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0504', TO_DATE('3/21/2005', 'MM/DD/YYYY'), TO_DATE('4/3/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0504'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0504', TO_DATE('3/21/2005', 'MM/DD/YYYY'), TO_DATE('4/3/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0504'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44090,11 +44093,11 @@
         <v>1049</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="I31" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0506', TO_DATE('5/5/2005', 'MM/DD/YYYY'), TO_DATE('5/20/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0506'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0506', TO_DATE('5/5/2005', 'MM/DD/YYYY'), TO_DATE('5/20/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0506'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44117,11 +44120,11 @@
         <v>1049</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="I32" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0509', TO_DATE('7/19/2005', 'MM/DD/YYYY'), TO_DATE('8/5/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0509'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0509', TO_DATE('7/19/2005', 'MM/DD/YYYY'), TO_DATE('8/5/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0509'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44144,11 +44147,11 @@
         <v>1049</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="I33" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0512', TO_DATE('10/3/2005', 'MM/DD/YYYY'), TO_DATE('10/9/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0512'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0512', TO_DATE('10/3/2005', 'MM/DD/YYYY'), TO_DATE('10/9/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0512'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44171,11 +44174,11 @@
         <v>1049</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="I34" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0604', TO_DATE('4/6/2006', 'MM/DD/YYYY'), TO_DATE('4/17/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0604'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0604', TO_DATE('4/6/2006', 'MM/DD/YYYY'), TO_DATE('4/17/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0604'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44198,11 +44201,11 @@
         <v>1049</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I35" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0606', TO_DATE('5/8/2006', 'MM/DD/YYYY'), TO_DATE('5/23/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0606'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0606', TO_DATE('5/8/2006', 'MM/DD/YYYY'), TO_DATE('5/23/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0606'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44225,11 +44228,11 @@
         <v>1049</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I36" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0607', TO_DATE('6/5/2006', 'MM/DD/YYYY'), TO_DATE('7/3/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0607'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0607', TO_DATE('6/5/2006', 'MM/DD/YYYY'), TO_DATE('7/3/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0607'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44252,11 +44255,11 @@
         <v>1049</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I37" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0608', TO_DATE('7/17/2006', 'MM/DD/YYYY'), TO_DATE('8/3/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0608'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0608', TO_DATE('7/17/2006', 'MM/DD/YYYY'), TO_DATE('8/3/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0608'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44279,11 +44282,11 @@
         <v>1049</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I38" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0706', TO_DATE('7/18/2007', 'MM/DD/YYYY'), TO_DATE('8/14/2007', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0706'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0706', TO_DATE('7/18/2007', 'MM/DD/YYYY'), TO_DATE('8/14/2007', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0706'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44306,11 +44309,11 @@
         <v>1049</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I39" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0908_LEGI', TO_DATE('9/1/2009', 'MM/DD/YYYY'), TO_DATE('9/30/2009', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0908'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0908_LEGI', TO_DATE('9/1/2009', 'MM/DD/YYYY'), TO_DATE('9/30/2009', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0908'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44333,11 +44336,11 @@
         <v>1049</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I40" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('OES0908_LEGII', TO_DATE('10/6/2009', 'MM/DD/YYYY'), TO_DATE('10/30/2009', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0908'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0908_LEGII', TO_DATE('10/6/2009', 'MM/DD/YYYY'), TO_DATE('10/30/2009', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0908'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44360,11 +44363,11 @@
         <v>1049</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I41" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0009', TO_DATE('7/19/2000', 'MM/DD/YYYY'), TO_DATE('8/4/2000', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0009'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC0009', TO_DATE('7/19/2000', 'MM/DD/YYYY'), TO_DATE('8/4/2000', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0009'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44387,11 +44390,11 @@
         <v>1049</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I42" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0011', TO_DATE('9/8/2000', 'MM/DD/YYYY'), TO_DATE('10/6/2000', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0011'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC0011', TO_DATE('9/8/2000', 'MM/DD/YYYY'), TO_DATE('10/6/2000', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0011'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44414,11 +44417,11 @@
         <v>1049</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I43" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0012', TO_DATE('10/9/2000', 'MM/DD/YYYY'), TO_DATE('11/5/2000', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0012'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC0012', TO_DATE('10/9/2000', 'MM/DD/YYYY'), TO_DATE('11/5/2000', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0012'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44441,11 +44444,11 @@
         <v>1049</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I44" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0108', TO_DATE('7/16/2001', 'MM/DD/YYYY'), TO_DATE('8/2/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0108'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC0108', TO_DATE('7/16/2001', 'MM/DD/YYYY'), TO_DATE('8/2/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0108'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44468,11 +44471,11 @@
         <v>1049</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I45" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0109_LEGI', TO_DATE('8/7/2001', 'MM/DD/YYYY'), TO_DATE('8/11/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0109'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC0109_LEGI', TO_DATE('8/7/2001', 'MM/DD/YYYY'), TO_DATE('8/11/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0109'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44495,11 +44498,11 @@
         <v>1049</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I46" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0109_LEGII', TO_DATE('8/12/2001', 'MM/DD/YYYY'), TO_DATE('8/27/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0109'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC0109_LEGII', TO_DATE('8/12/2001', 'MM/DD/YYYY'), TO_DATE('8/27/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0109'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44522,11 +44525,11 @@
         <v>1049</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I47" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0110', TO_DATE('9/10/2001', 'MM/DD/YYYY'), TO_DATE('10/1/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0110'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC0110', TO_DATE('9/10/2001', 'MM/DD/YYYY'), TO_DATE('10/1/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0110'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44549,11 +44552,11 @@
         <v>1049</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I48" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0111', TO_DATE('10/22/2001', 'MM/DD/YYYY'), TO_DATE('11/20/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0111'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC0111', TO_DATE('10/22/2001', 'MM/DD/YYYY'), TO_DATE('11/20/2001', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0111'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44576,11 +44579,11 @@
         <v>1049</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I49" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0201_LEGI', TO_DATE('1/21/2002', 'MM/DD/YYYY'), TO_DATE('3/25/2002', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0201'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC0201_LEGI', TO_DATE('1/21/2002', 'MM/DD/YYYY'), TO_DATE('3/25/2002', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0201'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44603,11 +44606,11 @@
         <v>1049</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I50" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0201_LEGII', TO_DATE('1/21/2002', 'MM/DD/YYYY'), TO_DATE('3/25/2002', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0201'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC0201_LEGII', TO_DATE('1/21/2002', 'MM/DD/YYYY'), TO_DATE('3/25/2002', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0201'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44630,11 +44633,11 @@
         <v>1049</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I51" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0207', TO_DATE('9/8/2002', 'MM/DD/YYYY'), TO_DATE('10/7/2002', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0207'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC0207', TO_DATE('9/8/2002', 'MM/DD/YYYY'), TO_DATE('10/7/2002', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0207'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44657,11 +44660,11 @@
         <v>1049</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I52" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC9905', TO_DATE('4/26/1999', 'MM/DD/YYYY'), TO_DATE('5/9/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9905'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC9905', TO_DATE('4/26/1999', 'MM/DD/YYYY'), TO_DATE('5/9/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9905'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44684,11 +44687,11 @@
         <v>1049</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I53" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC9906', TO_DATE('5/15/1999', 'MM/DD/YYYY'), TO_DATE('5/31/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9906'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC9906', TO_DATE('5/15/1999', 'MM/DD/YYYY'), TO_DATE('5/31/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9906'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44711,11 +44714,11 @@
         <v>1049</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I54" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC9908', TO_DATE('7/15/1999', 'MM/DD/YYYY'), TO_DATE('8/2/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9908'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC9908', TO_DATE('7/15/1999', 'MM/DD/YYYY'), TO_DATE('8/2/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9908'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44738,11 +44741,11 @@
         <v>1049</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I55" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC9909_LEGI', TO_DATE('8/13/1999', 'MM/DD/YYYY'), TO_DATE('8/29/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9909'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC9909_LEGI', TO_DATE('8/13/1999', 'MM/DD/YYYY'), TO_DATE('8/29/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9909'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44765,11 +44768,11 @@
         <v>1049</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I56" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC9909_LEGII', TO_DATE('8/30/1999', 'MM/DD/YYYY'), TO_DATE('9/7/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9909'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC9909_LEGII', TO_DATE('8/30/1999', 'MM/DD/YYYY'), TO_DATE('9/7/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9909'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44792,11 +44795,11 @@
         <v>1049</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I57" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC9910', TO_DATE('10/6/1999', 'MM/DD/YYYY'), TO_DATE('11/4/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9910'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC9910', TO_DATE('10/6/1999', 'MM/DD/YYYY'), TO_DATE('11/4/1999', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC9910'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44822,11 +44825,11 @@
         <v>1049</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I58" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('TC0005', TO_DATE('5/8/2000', 'MM/DD/YYYY'), TO_DATE('5/17/2000', 'MM/DD/YYYY'), 'Leg dates were made up for testing purposes based on the dates in the cast files', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0005'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('TC0005', TO_DATE('5/8/2000', 'MM/DD/YYYY'), TO_DATE('5/17/2000', 'MM/DD/YYYY'), 'Leg dates were made up for testing purposes based on the dates in the cast files', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'TC0005'), (select vessel_id from ccd_vessels where vessel_name = 'Townsend Cromwell'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -44852,11 +44855,11 @@
         <v>1049</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I59" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('RL-17-05 Leg 1', TO_DATE('8/17/2017', 'MM/DD/YYYY'), TO_DATE('9/5/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('RL-17-05 Leg 1', TO_DATE('8/17/2017', 'MM/DD/YYYY'), TO_DATE('9/5/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -44882,11 +44885,11 @@
         <v>1049</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I60" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('RL-17-05 Leg 2', TO_DATE('9/11/2017', 'MM/DD/YYYY'), TO_DATE('9/30/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('RL-17-05 Leg 2', TO_DATE('9/11/2017', 'MM/DD/YYYY'), TO_DATE('9/30/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -44912,11 +44915,11 @@
         <v>1049</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I61" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('RL-17-05 Leg 3', TO_DATE('10/1/2017', 'MM/DD/YYYY'), TO_DATE('10/10/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('RL-17-05 Leg 3', TO_DATE('10/1/2017', 'MM/DD/YYYY'), TO_DATE('10/10/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -44942,11 +44945,11 @@
         <v>1049</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I62" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('RL-17-05 Leg 4', TO_DATE('10/16/2017', 'MM/DD/YYYY'), TO_DATE('11/9/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('RL-17-05 Leg 4', TO_DATE('10/16/2017', 'MM/DD/YYYY'), TO_DATE('11/9/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -44972,11 +44975,11 @@
         <v>1049</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I63" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('RL-17-05 Leg 5', TO_DATE('11/15/2017', 'MM/DD/YYYY'), TO_DATE('12/9/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('RL-17-05 Leg 5', TO_DATE('11/15/2017', 'MM/DD/YYYY'), TO_DATE('12/9/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via online Ship Schedule (https://sdat.noaa.gov/Account/Login?ReturnUrl=%2FHome%2FSchedule)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -45002,11 +45005,11 @@
         <v>1049</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I64" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-17-06 Leg 1', TO_DATE('7/6/2017', 'MM/DD/YYYY'), TO_DATE('8/2/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-17-06 Leg 1', TO_DATE('7/6/2017', 'MM/DD/YYYY'), TO_DATE('8/2/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -45032,11 +45035,11 @@
         <v>1049</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I65" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-17-06 Leg 2', TO_DATE('8/8/2017', 'MM/DD/YYYY'), TO_DATE('9/5/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-17-06 Leg 2', TO_DATE('8/8/2017', 'MM/DD/YYYY'), TO_DATE('9/5/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -45062,11 +45065,11 @@
         <v>1049</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I66" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-17-06 Leg 3', TO_DATE('9/11/2017', 'MM/DD/YYYY'), TO_DATE('10/10/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-17-06 Leg 3', TO_DATE('9/11/2017', 'MM/DD/YYYY'), TO_DATE('10/10/2017', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -45092,11 +45095,11 @@
         <v>1049</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I67" s="5" t="str">
         <f t="shared" ref="I67:I69" si="1">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B67, "'", "''"), "', TO_DATE('", C67, "', 'MM/DD/YYYY'), TO_DATE('", D67, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E67, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F67, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A67, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G67, "'", "''"), "'), '", H67, "');")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-19-01', TO_DATE('4/3/2019', 'MM/DD/YYYY'), TO_DATE('4/12/2019', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-19-01', TO_DATE('4/3/2019', 'MM/DD/YYYY'), TO_DATE('4/12/2019', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -45122,11 +45125,11 @@
         <v>1049</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I68" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-18-03', TO_DATE('7/8/2018', 'MM/DD/YYYY'), TO_DATE('7/31/2018', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-18-03'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-18-03', TO_DATE('7/8/2018', 'MM/DD/YYYY'), TO_DATE('7/31/2018', 'MM/DD/YYYY'), 'Leg dates were retrieved via SciOps Who''s Where calendar', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-18-03'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -45152,11 +45155,11 @@
         <v>1049</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I69" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-19-06', TO_DATE('9/11/2019', 'MM/DD/YYYY'), TO_DATE('9/29/2019', 'MM/DD/YYYY'), 'Leg dates retrieved from project report', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-19-06', TO_DATE('9/11/2019', 'MM/DD/YYYY'), TO_DATE('9/29/2019', 'MM/DD/YYYY'), 'Leg dates retrieved from project report', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -45191,11 +45194,11 @@
         <v>1049</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I72" s="5" t="str">
         <f t="shared" ref="I72:I78" si="2">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B72, "'", "''"), "', TO_DATE('", C72, "', 'MM/DD/YYYY'), TO_DATE('", D72, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E72, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F72, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A72, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G72, "'", "''"), "'), '", H72, "');")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-14-01', TO_DATE('3/18/2014', 'MM/DD/YYYY'), TO_DATE('3/27/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-14-01', TO_DATE('3/18/2014', 'MM/DD/YYYY'), TO_DATE('3/27/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -45221,11 +45224,11 @@
         <v>1049</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I73" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-14-02', TO_DATE('4/6/2014', 'MM/DD/YYYY'), TO_DATE('4/18/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-14-02', TO_DATE('4/6/2014', 'MM/DD/YYYY'), TO_DATE('4/18/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -45251,11 +45254,11 @@
         <v>1049</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I74" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-14-04 Leg 1', TO_DATE('6/21/2014', 'MM/DD/YYYY'), TO_DATE('7/1/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-14-04 Leg 1', TO_DATE('6/21/2014', 'MM/DD/YYYY'), TO_DATE('7/1/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -45281,11 +45284,11 @@
         <v>1049</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I75" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-14-04 Leg 2', TO_DATE('7/8/2014', 'MM/DD/YYYY'), TO_DATE('7/19/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-14-04 Leg 2', TO_DATE('7/8/2014', 'MM/DD/YYYY'), TO_DATE('7/19/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -45311,11 +45314,11 @@
         <v>1049</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I76" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-14-05', TO_DATE('7/25/2014', 'MM/DD/YYYY'), TO_DATE('8/23/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-05'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-14-05', TO_DATE('7/25/2014', 'MM/DD/YYYY'), TO_DATE('8/23/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-05'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -45341,11 +45344,11 @@
         <v>1049</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I77" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-14-06', TO_DATE('8/31/2014', 'MM/DD/YYYY'), TO_DATE('9/18/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-14-06', TO_DATE('8/31/2014', 'MM/DD/YYYY'), TO_DATE('9/18/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -45371,11 +45374,11 @@
         <v>1049</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I78" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-14-07', TO_DATE('10/2/2014', 'MM/DD/YYYY'), TO_DATE('10/27/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-07'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-14-07', TO_DATE('10/2/2014', 'MM/DD/YYYY'), TO_DATE('10/27/2014', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-14-07'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -45401,11 +45404,11 @@
         <v>1049</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I81" s="5" t="str">
         <f>CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B81, "'", "''"), "', TO_DATE('", C81, "', 'MM/DD/YYYY'), TO_DATE('", D81, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E81, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F81, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A81, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G81, "'", "''"), "'), '", H81, "');")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-15-01', TO_DATE('4/3/2015', 'MM/DD/YYYY'), TO_DATE('4/14/2015', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-15-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-15-01', TO_DATE('4/3/2015', 'MM/DD/YYYY'), TO_DATE('4/14/2015', 'MM/DD/YYYY'), 'Leg dates were retrieved from https://sdat.noaa.gov/DataManagement/Tracking#', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-15-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -45436,11 +45439,11 @@
         <v>1049</v>
       </c>
       <c r="H87" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I87" s="5" t="str">
         <f t="shared" ref="I87:I122" si="3">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B87, "'", "''"), "', TO_DATE('", C87, "', 'MM/DD/YYYY'), TO_DATE('", D87, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E87, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F87, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A87, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G87, "'", "''"), "'), '", H87, "');")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-20-04 Leg 1', TO_DATE('3/20/2020', 'MM/DD/YYYY'), TO_DATE('4/15/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-20-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-20-04 Leg 1', TO_DATE('3/20/2020', 'MM/DD/YYYY'), TO_DATE('4/15/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-20-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -45466,11 +45469,11 @@
         <v>1049</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I88" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-20-05 Leg 1', TO_DATE('4/10/2020', 'MM/DD/YYYY'), TO_DATE('4/25/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-20-05'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-20-05 Leg 1', TO_DATE('4/10/2020', 'MM/DD/YYYY'), TO_DATE('4/25/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-20-05'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -45496,11 +45499,11 @@
         <v>1049</v>
       </c>
       <c r="H89" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I89" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-01 Leg 1', TO_DATE('10/15/2020', 'MM/DD/YYYY'), TO_DATE('10/30/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-21-01 Leg 1', TO_DATE('10/15/2020', 'MM/DD/YYYY'), TO_DATE('10/30/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -45526,11 +45529,11 @@
         <v>1049</v>
       </c>
       <c r="H90" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I90" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-01 Leg 2', TO_DATE('11/5/2020', 'MM/DD/YYYY'), TO_DATE('11/20/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-21-01 Leg 2', TO_DATE('11/5/2020', 'MM/DD/YYYY'), TO_DATE('11/20/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -45556,11 +45559,11 @@
         <v>1049</v>
       </c>
       <c r="H91" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I91" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-03', TO_DATE('11/15/2020', 'MM/DD/YYYY'), TO_DATE('12/1/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-03'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-21-03', TO_DATE('11/15/2020', 'MM/DD/YYYY'), TO_DATE('12/1/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-03'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -45586,11 +45589,11 @@
         <v>1049</v>
       </c>
       <c r="H92" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I92" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-04 Leg 1', TO_DATE('11/22/2020', 'MM/DD/YYYY'), TO_DATE('11/28/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-21-04 Leg 1', TO_DATE('11/22/2020', 'MM/DD/YYYY'), TO_DATE('11/28/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -45616,11 +45619,11 @@
         <v>1049</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I93" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-04 Leg 2', TO_DATE('11/30/2020', 'MM/DD/YYYY'), TO_DATE('12/10/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-21-04 Leg 2', TO_DATE('11/30/2020', 'MM/DD/YYYY'), TO_DATE('12/10/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-04'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -45646,11 +45649,11 @@
         <v>1049</v>
       </c>
       <c r="H94" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I94" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-21-06', TO_DATE('3/15/2021', 'MM/DD/YYYY'), TO_DATE('3/30/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-06'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI-21-06', TO_DATE('3/15/2021', 'MM/DD/YYYY'), TO_DATE('3/30/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-06'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -45676,11 +45679,11 @@
         <v>1049</v>
       </c>
       <c r="H95" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I95" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-21-07 Leg 1', TO_DATE('3/27/2021', 'MM/DD/YYYY'), TO_DATE('4/15/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-07'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI-21-07 Leg 1', TO_DATE('3/27/2021', 'MM/DD/YYYY'), TO_DATE('4/15/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-07'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -45706,11 +45709,11 @@
         <v>1049</v>
       </c>
       <c r="H96" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I96" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-21-07 Leg 2', TO_DATE('4/18/2021', 'MM/DD/YYYY'), TO_DATE('4/30/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-07'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI-21-07 Leg 2', TO_DATE('4/18/2021', 'MM/DD/YYYY'), TO_DATE('4/30/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-07'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -45736,11 +45739,11 @@
         <v>1049</v>
       </c>
       <c r="H97" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I97" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-21-08 Leg 1', TO_DATE('4/28/2021', 'MM/DD/YYYY'), TO_DATE('5/23/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI-21-08 Leg 1', TO_DATE('4/28/2021', 'MM/DD/YYYY'), TO_DATE('5/23/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -45766,11 +45769,11 @@
         <v>1049</v>
       </c>
       <c r="H98" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I98" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-21-08 Leg 2', TO_DATE('5/25/2021', 'MM/DD/YYYY'), TO_DATE('6/17/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI-21-08 Leg 2', TO_DATE('5/25/2021', 'MM/DD/YYYY'), TO_DATE('6/17/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-21-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -45796,11 +45799,11 @@
         <v>1049</v>
       </c>
       <c r="H99" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I99" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-20-08 Leg 1', TO_DATE('6/10/2020', 'MM/DD/YYYY'), TO_DATE('6/29/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI-20-08 Leg 1', TO_DATE('6/10/2020', 'MM/DD/YYYY'), TO_DATE('6/29/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -45826,11 +45829,11 @@
         <v>1049</v>
       </c>
       <c r="H100" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I100" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-20-08 Leg 2', TO_DATE('7/2/2020', 'MM/DD/YYYY'), TO_DATE('7/26/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI-20-08 Leg 2', TO_DATE('7/2/2020', 'MM/DD/YYYY'), TO_DATE('7/26/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -45856,11 +45859,11 @@
         <v>1049</v>
       </c>
       <c r="H101" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I101" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-20-09 Leg 1', TO_DATE('7/20/2020', 'MM/DD/YYYY'), TO_DATE('8/12/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-09'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI-20-09 Leg 1', TO_DATE('7/20/2020', 'MM/DD/YYYY'), TO_DATE('8/12/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-09'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -45886,11 +45889,11 @@
         <v>1049</v>
       </c>
       <c r="H102" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I102" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-20-09 Leg 2', TO_DATE('8/16/2020', 'MM/DD/YYYY'), TO_DATE('9/2/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-09'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI-20-09 Leg 2', TO_DATE('8/16/2020', 'MM/DD/YYYY'), TO_DATE('9/2/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-09'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -45916,11 +45919,11 @@
         <v>1049</v>
       </c>
       <c r="H103" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I103" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-20-10 Leg 1', TO_DATE('6/14/2020', 'MM/DD/YYYY'), TO_DATE('7/30/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-10'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI-20-10 Leg 1', TO_DATE('6/14/2020', 'MM/DD/YYYY'), TO_DATE('7/30/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-10'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -45946,11 +45949,11 @@
         <v>1049</v>
       </c>
       <c r="H104" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I104" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-06 Leg 1', TO_DATE('1/12/2021', 'MM/DD/YYYY'), TO_DATE('1/31/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-21-06 Leg 1', TO_DATE('1/12/2021', 'MM/DD/YYYY'), TO_DATE('1/31/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -45976,11 +45979,11 @@
         <v>1049</v>
       </c>
       <c r="H105" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I105" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-06 Leg 2', TO_DATE('2/3/2021', 'MM/DD/YYYY'), TO_DATE('2/25/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-21-06 Leg 2', TO_DATE('2/3/2021', 'MM/DD/YYYY'), TO_DATE('2/25/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -46006,11 +46009,11 @@
         <v>1049</v>
       </c>
       <c r="H106" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I106" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-07', TO_DATE('1/30/2021', 'MM/DD/YYYY'), TO_DATE('3/6/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-07'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-21-07', TO_DATE('1/30/2021', 'MM/DD/YYYY'), TO_DATE('3/6/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-07'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -46036,11 +46039,11 @@
         <v>1049</v>
       </c>
       <c r="H107" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I107" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-08 Leg 1', TO_DATE('3/2/2021', 'MM/DD/YYYY'), TO_DATE('3/23/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-08'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-21-08 Leg 1', TO_DATE('3/2/2021', 'MM/DD/YYYY'), TO_DATE('3/23/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-08'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -46066,11 +46069,11 @@
         <v>1049</v>
       </c>
       <c r="H108" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I108" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-08 Leg 2', TO_DATE('3/26/2021', 'MM/DD/YYYY'), TO_DATE('4/12/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-08'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-21-08 Leg 2', TO_DATE('3/26/2021', 'MM/DD/YYYY'), TO_DATE('4/12/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-08'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -46096,11 +46099,11 @@
         <v>1049</v>
       </c>
       <c r="H109" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I109" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-09 Leg 1', TO_DATE('5/11/2021', 'MM/DD/YYYY'), TO_DATE('5/30/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-09'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-21-09 Leg 1', TO_DATE('5/11/2021', 'MM/DD/YYYY'), TO_DATE('5/30/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-09'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -46126,11 +46129,11 @@
         <v>1049</v>
       </c>
       <c r="H110" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I110" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-21-09 Leg 2', TO_DATE('6/2/2021', 'MM/DD/YYYY'), TO_DATE('6/19/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-09'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-21-09 Leg 2', TO_DATE('6/2/2021', 'MM/DD/YYYY'), TO_DATE('6/19/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 1)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-09'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -46156,11 +46159,11 @@
         <v>1049</v>
       </c>
       <c r="H111" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I111" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-19-04 Leg 1', TO_DATE('6/1/2019', 'MM/DD/YYYY'), TO_DATE('6/15/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-04'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-19-04 Leg 1', TO_DATE('6/1/2019', 'MM/DD/YYYY'), TO_DATE('6/15/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-04'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -46186,11 +46189,11 @@
         <v>1049</v>
       </c>
       <c r="H112" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I112" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-19-04 Leg 2', TO_DATE('6/19/2019', 'MM/DD/YYYY'), TO_DATE('7/12/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-04'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-19-04 Leg 2', TO_DATE('6/19/2019', 'MM/DD/YYYY'), TO_DATE('7/12/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-04'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -46216,11 +46219,11 @@
         <v>1049</v>
       </c>
       <c r="H113" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I113" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-19-05 Leg 1', TO_DATE('7/14/2019', 'MM/DD/YYYY'), TO_DATE('7/31/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-05'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-19-05 Leg 1', TO_DATE('7/14/2019', 'MM/DD/YYYY'), TO_DATE('7/31/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-05'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -46246,11 +46249,11 @@
         <v>1049</v>
       </c>
       <c r="H114" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I114" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-19-05 Leg 2', TO_DATE('8/2/2019', 'MM/DD/YYYY'), TO_DATE('8/15/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-05'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-19-05 Leg 2', TO_DATE('8/2/2019', 'MM/DD/YYYY'), TO_DATE('8/15/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-05'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -46276,11 +46279,11 @@
         <v>1049</v>
       </c>
       <c r="H115" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I115" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-19-01 Leg 1', TO_DATE('10/15/2018', 'MM/DD/YYYY'), TO_DATE('11/2/2018', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-19-01'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI-19-01 Leg 1', TO_DATE('10/15/2018', 'MM/DD/YYYY'), TO_DATE('11/2/2018', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-19-01'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -46306,11 +46309,11 @@
         <v>1049</v>
       </c>
       <c r="H116" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I116" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-19-01 Leg 2', TO_DATE('11/5/2018', 'MM/DD/YYYY'), TO_DATE('11/29/2018', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-19-01'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI-19-01 Leg 2', TO_DATE('11/5/2018', 'MM/DD/YYYY'), TO_DATE('11/29/2018', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-19-01'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -46336,11 +46339,11 @@
         <v>1049</v>
       </c>
       <c r="H117" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I117" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-19-02 Leg 1', TO_DATE('11/20/2018', 'MM/DD/YYYY'), TO_DATE('12/10/2018', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-19-02'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI-19-02 Leg 1', TO_DATE('11/20/2018', 'MM/DD/YYYY'), TO_DATE('12/10/2018', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-19-02'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -46366,11 +46369,11 @@
         <v>1049</v>
       </c>
       <c r="H118" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I118" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('HI-19-02 Leg 2', TO_DATE('12/12/2018', 'MM/DD/YYYY'), TO_DATE('12/30/2018', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-19-02'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI-19-02 Leg 2', TO_DATE('12/12/2018', 'MM/DD/YYYY'), TO_DATE('12/30/2018', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 3)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-19-02'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -46396,11 +46399,11 @@
         <v>1049</v>
       </c>
       <c r="H119" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I119" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-22-01 Leg 1', TO_DATE('10/21/2021', 'MM/DD/YYYY'), TO_DATE('11/13/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-22-01 Leg 1', TO_DATE('10/21/2021', 'MM/DD/YYYY'), TO_DATE('11/13/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -46426,11 +46429,11 @@
         <v>1049</v>
       </c>
       <c r="H120" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I120" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-22-01 Leg 2', TO_DATE('11/15/2021', 'MM/DD/YYYY'), TO_DATE('12/4/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-22-01 Leg 2', TO_DATE('11/15/2021', 'MM/DD/YYYY'), TO_DATE('12/4/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -46456,11 +46459,11 @@
         <v>1049</v>
       </c>
       <c r="H121" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I121" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-22-02 Leg 1', TO_DATE('11/30/2021', 'MM/DD/YYYY'), TO_DATE('12/15/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-22-02 Leg 1', TO_DATE('11/30/2021', 'MM/DD/YYYY'), TO_DATE('12/15/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -46486,11 +46489,11 @@
         <v>1049</v>
       </c>
       <c r="H122" s="6" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="I122" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, UTC_TZ_OFFSET) values ('SE-22-02 Leg 2', TO_DATE('12/17/2021', 'MM/DD/YYYY'), TO_DATE('1/12/2022', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-22-02 Leg 2', TO_DATE('12/17/2021', 'MM/DD/YYYY'), TO_DATE('1/12/2022', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data loading scripts
</commit_message>
<xml_diff>
--- a/docs/Cruise_Leg_DDL_DML_generator.xlsx
+++ b/docs/Cruise_Leg_DDL_DML_generator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Vessels" sheetId="10" r:id="rId1"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4953" uniqueCount="2027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4958" uniqueCount="2029">
   <si>
     <t>Cruise Name</t>
   </si>
@@ -6219,6 +6219,12 @@
   </si>
   <si>
     <t>US/Hawaii</t>
+  </si>
+  <si>
+    <t>2019 MOUSS Data Set</t>
+  </si>
+  <si>
+    <t>https://inport.nmfs.noaa.gov/inport/item/99999</t>
   </si>
 </sst>
 </file>
@@ -25733,8 +25739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43248,9 +43254,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H87" sqref="H87:H122"/>
+      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54920,8 +54926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55097,9 +55103,24 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2027</v>
+      </c>
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2028</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2018</v>
+      </c>
+      <c r="H9" t="s">
+        <v>179</v>
+      </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_data_sets (DATA_SET_DESC, DATA_SET_TYPE_ID, DATA_SET_DOI, DATA_SET_INPORT_URL, DATA_SET_ACCESS_URL, DATA_SET_ARCHIVE_URL, CRUISE_LEG_ID, DATA_SET_STATUS_ID) values ('', (SELECT DATA_SET_TYPE_ID FROM CCD_DATA_SET_TYPES WHERE DATA_SET_TYPE_NAME = ''), '', '', '', '', (SELECT CRUISE_LEG_ID FROM CCD_CRUISE_LEGS where leg_name = ''), (SELECT DATA_SET_STATUS_ID FROM CCD_DATA_SET_STATUS where status_code = ''));</v>
+        <v>insert into ccd_data_sets (DATA_SET_DESC, DATA_SET_TYPE_ID, DATA_SET_DOI, DATA_SET_INPORT_URL, DATA_SET_ACCESS_URL, DATA_SET_ARCHIVE_URL, CRUISE_LEG_ID, DATA_SET_STATUS_ID) values ('2019 MOUSS Data Set', (SELECT DATA_SET_TYPE_ID FROM CCD_DATA_SET_TYPES WHERE DATA_SET_TYPE_NAME = 'MOUSS Video'), '', 'https://inport.nmfs.noaa.gov/inport/item/99999', '', '', (SELECT CRUISE_LEG_ID FROM CCD_CRUISE_LEGS where leg_name = 'SE-19-06'), (SELECT DATA_SET_STATUS_ID FROM CCD_DATA_SET_STATUS where status_code = 'QC'));</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implementing TZ_NAME DVM criteria
</commit_message>
<xml_diff>
--- a/docs/Cruise_Leg_DDL_DML_generator.xlsx
+++ b/docs/Cruise_Leg_DDL_DML_generator.xlsx
@@ -139,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5501" uniqueCount="2126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5501" uniqueCount="2133">
   <si>
     <t>Cruise Name</t>
   </si>
@@ -6181,9 +6181,6 @@
   </si>
   <si>
     <t>SE1906</t>
-  </si>
-  <si>
-    <t>-10:00</t>
   </si>
   <si>
     <t>TZ_NAME</t>
@@ -6518,6 +6515,30 @@
   </si>
   <si>
     <t>Don't include in test category 5 (the cruise is deleted)</t>
+  </si>
+  <si>
+    <t>Etc/GMT+10</t>
+  </si>
+  <si>
+    <t>ASDF JKL;</t>
+  </si>
+  <si>
+    <t>+09:00</t>
+  </si>
+  <si>
+    <t>Hawaii Standard Time</t>
+  </si>
+  <si>
+    <t>Eastern US Time</t>
+  </si>
+  <si>
+    <t>Mountain/Pacific Time</t>
+  </si>
+  <si>
+    <t>Something else</t>
+  </si>
+  <si>
+    <t>IDK What is this field?</t>
   </si>
 </sst>
 </file>
@@ -6651,7 +6672,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -6683,6 +6704,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -43352,8 +43374,8 @@
   <dimension ref="A1:K153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A131" sqref="A131"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43388,13 +43410,13 @@
         <v>1716</v>
       </c>
       <c r="H1" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="I1" t="s">
         <v>109</v>
       </c>
       <c r="J1" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43417,7 +43439,7 @@
         <v>1040</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I2" s="5" t="str">
         <f>CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B2, "'", "''"), "', TO_DATE('", C2, "', 'MM/DD/YYYY'), TO_DATE('", D2, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E2, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F2, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A2, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G2, "'", "''"), "'), '", H2, "');")</f>
@@ -43444,11 +43466,11 @@
         <v>1040</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>2014</v>
+        <v>2125</v>
       </c>
       <c r="I3" s="5" t="str">
         <f t="shared" ref="I3:I66" si="0">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B3, "'", "''"), "', TO_DATE('", C3, "', 'MM/DD/YYYY'), TO_DATE('", D3, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E3, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F3, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A3, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G3, "'", "''"), "'), '", H3, "');")</f>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-18-06', TO_DATE('10/17/2018', 'MM/DD/YYYY'), TO_DATE('10/31/2018', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-18-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-18-06', TO_DATE('10/17/2018', 'MM/DD/YYYY'), TO_DATE('10/31/2018', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-18-06'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Etc/GMT+10');</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43471,11 +43493,11 @@
         <v>1040</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>2014</v>
+        <v>2125</v>
       </c>
       <c r="I4" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-17-02', TO_DATE('3/1/2017', 'MM/DD/YYYY'), TO_DATE('3/15/2017', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-17-02', TO_DATE('3/1/2017', 'MM/DD/YYYY'), TO_DATE('3/15/2017', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-17-02'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Etc/GMT+10');</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43498,11 +43520,11 @@
         <v>1040</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>2014</v>
+        <v>2125</v>
       </c>
       <c r="I5" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-15-01', TO_DATE('4/3/2015', 'MM/DD/YYYY'), TO_DATE('4/14/2015', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-15-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-15-01', TO_DATE('4/3/2015', 'MM/DD/YYYY'), TO_DATE('4/14/2015', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-15-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Etc/GMT+10');</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -43525,7 +43547,7 @@
         <v>1040</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I6" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43552,7 +43574,7 @@
         <v>1040</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I7" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43579,7 +43601,7 @@
         <v>1040</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I8" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43606,7 +43628,7 @@
         <v>1040</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I9" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43633,7 +43655,7 @@
         <v>1040</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I10" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43660,7 +43682,7 @@
         <v>1040</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I11" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43687,7 +43709,7 @@
         <v>1040</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I12" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43714,7 +43736,7 @@
         <v>1040</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I13" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43741,7 +43763,7 @@
         <v>1040</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I14" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43768,7 +43790,7 @@
         <v>1040</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I15" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43795,7 +43817,7 @@
         <v>1040</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I16" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43822,7 +43844,7 @@
         <v>1040</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I17" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43849,7 +43871,7 @@
         <v>1040</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I18" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43876,7 +43898,7 @@
         <v>1040</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I19" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43903,7 +43925,7 @@
         <v>1040</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I20" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43930,7 +43952,7 @@
         <v>1040</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I21" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43957,7 +43979,7 @@
         <v>1040</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I22" s="5" t="str">
         <f t="shared" si="0"/>
@@ -43984,11 +44006,11 @@
         <v>1040</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>2014</v>
+        <v>2125</v>
       </c>
       <c r="I23" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI1001_LEGIII', TO_DATE('3/27/2010', 'MM/DD/YYYY'), TO_DATE('4/24/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1001'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI1001_LEGIII', TO_DATE('3/27/2010', 'MM/DD/YYYY'), TO_DATE('4/24/2010', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1001'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Etc/GMT+10');</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44011,11 +44033,11 @@
         <v>1040</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>2014</v>
+        <v>2125</v>
       </c>
       <c r="I24" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0304', TO_DATE('5/13/2003', 'MM/DD/YYYY'), TO_DATE('5/28/2003', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0304'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0304', TO_DATE('5/13/2003', 'MM/DD/YYYY'), TO_DATE('5/28/2003', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0304'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Etc/GMT+10');</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44038,11 +44060,11 @@
         <v>1040</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>2014</v>
+        <v>2125</v>
       </c>
       <c r="I25" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0306', TO_DATE('7/12/2003', 'MM/DD/YYYY'), TO_DATE('8/17/2003', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0306'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0306', TO_DATE('7/12/2003', 'MM/DD/YYYY'), TO_DATE('8/17/2003', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0306'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Etc/GMT+10');</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44065,11 +44087,11 @@
         <v>1040</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>2014</v>
+        <v>2125</v>
       </c>
       <c r="I26" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0407', TO_DATE('5/30/2004', 'MM/DD/YYYY'), TO_DATE('6/14/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0407'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0407', TO_DATE('5/30/2004', 'MM/DD/YYYY'), TO_DATE('6/14/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0407'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Etc/GMT+10');</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44092,11 +44114,11 @@
         <v>1040</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>2014</v>
+        <v>2125</v>
       </c>
       <c r="I27" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0410', TO_DATE('7/30/2004', 'MM/DD/YYYY'), TO_DATE('8/16/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0410'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0410', TO_DATE('7/30/2004', 'MM/DD/YYYY'), TO_DATE('8/16/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0410'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Etc/GMT+10');</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44119,11 +44141,11 @@
         <v>1040</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>2014</v>
+        <v>2125</v>
       </c>
       <c r="I28" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0411_LEGI', TO_DATE('8/7/2004', 'MM/DD/YYYY'), TO_DATE('9/7/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0411'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0411_LEGI', TO_DATE('8/7/2004', 'MM/DD/YYYY'), TO_DATE('9/7/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0411'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Etc/GMT+10');</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44146,11 +44168,11 @@
         <v>1040</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>2014</v>
+        <v>2125</v>
       </c>
       <c r="I29" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0411_LEGII', TO_DATE('9/8/2004', 'MM/DD/YYYY'), TO_DATE('9/13/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0411'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0411_LEGII', TO_DATE('9/8/2004', 'MM/DD/YYYY'), TO_DATE('9/13/2004', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0411'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Etc/GMT+10');</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44173,11 +44195,11 @@
         <v>1040</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>2014</v>
+        <v>2125</v>
       </c>
       <c r="I30" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0504', TO_DATE('3/21/2005', 'MM/DD/YYYY'), TO_DATE('4/3/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0504'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0504', TO_DATE('3/21/2005', 'MM/DD/YYYY'), TO_DATE('4/3/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0504'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Etc/GMT+10');</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44200,11 +44222,11 @@
         <v>1040</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>2014</v>
+        <v>2125</v>
       </c>
       <c r="I31" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0506', TO_DATE('5/5/2005', 'MM/DD/YYYY'), TO_DATE('5/20/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0506'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0506', TO_DATE('5/5/2005', 'MM/DD/YYYY'), TO_DATE('5/20/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0506'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Etc/GMT+10');</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44227,11 +44249,11 @@
         <v>1040</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>2014</v>
+        <v>2125</v>
       </c>
       <c r="I32" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0509', TO_DATE('7/19/2005', 'MM/DD/YYYY'), TO_DATE('8/5/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0509'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0509', TO_DATE('7/19/2005', 'MM/DD/YYYY'), TO_DATE('8/5/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0509'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Etc/GMT+10');</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44254,11 +44276,11 @@
         <v>1040</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>2014</v>
+        <v>2125</v>
       </c>
       <c r="I33" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0512', TO_DATE('10/3/2005', 'MM/DD/YYYY'), TO_DATE('10/9/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0512'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0512', TO_DATE('10/3/2005', 'MM/DD/YYYY'), TO_DATE('10/9/2005', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0512'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Etc/GMT+10');</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44281,11 +44303,11 @@
         <v>1040</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>2014</v>
+        <v>2125</v>
       </c>
       <c r="I34" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0604', TO_DATE('4/6/2006', 'MM/DD/YYYY'), TO_DATE('4/17/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0604'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '-10:00');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0604', TO_DATE('4/6/2006', 'MM/DD/YYYY'), TO_DATE('4/17/2006', 'MM/DD/YYYY'), '', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0604'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Etc/GMT+10');</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -44308,7 +44330,7 @@
         <v>1040</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I35" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44335,7 +44357,7 @@
         <v>1040</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I36" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44362,7 +44384,7 @@
         <v>1040</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I37" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44389,7 +44411,7 @@
         <v>1040</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I38" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44416,7 +44438,7 @@
         <v>1040</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I39" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44443,7 +44465,7 @@
         <v>1040</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I40" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44470,7 +44492,7 @@
         <v>1040</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I41" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44497,7 +44519,7 @@
         <v>1040</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I42" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44524,7 +44546,7 @@
         <v>1040</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I43" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44551,7 +44573,7 @@
         <v>1040</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I44" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44578,7 +44600,7 @@
         <v>1040</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I45" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44605,7 +44627,7 @@
         <v>1040</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I46" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44632,7 +44654,7 @@
         <v>1040</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I47" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44659,7 +44681,7 @@
         <v>1040</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I48" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44686,7 +44708,7 @@
         <v>1040</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I49" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44713,7 +44735,7 @@
         <v>1040</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I50" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44740,7 +44762,7 @@
         <v>1040</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I51" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44767,7 +44789,7 @@
         <v>1040</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I52" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44794,7 +44816,7 @@
         <v>1040</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I53" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44821,7 +44843,7 @@
         <v>1040</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I54" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44848,7 +44870,7 @@
         <v>1040</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I55" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44875,7 +44897,7 @@
         <v>1040</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I56" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44902,7 +44924,7 @@
         <v>1040</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I57" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44932,7 +44954,7 @@
         <v>1040</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I58" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44962,7 +44984,7 @@
         <v>1040</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I59" s="5" t="str">
         <f t="shared" si="0"/>
@@ -44992,7 +45014,7 @@
         <v>1040</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I60" s="5" t="str">
         <f t="shared" si="0"/>
@@ -45022,7 +45044,7 @@
         <v>1040</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I61" s="5" t="str">
         <f t="shared" si="0"/>
@@ -45052,7 +45074,7 @@
         <v>1040</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I62" s="5" t="str">
         <f t="shared" si="0"/>
@@ -45082,7 +45104,7 @@
         <v>1040</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I63" s="5" t="str">
         <f t="shared" si="0"/>
@@ -45112,7 +45134,7 @@
         <v>1040</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I64" s="5" t="str">
         <f t="shared" si="0"/>
@@ -45142,7 +45164,7 @@
         <v>1040</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I65" s="5" t="str">
         <f t="shared" si="0"/>
@@ -45172,7 +45194,7 @@
         <v>1040</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I66" s="5" t="str">
         <f t="shared" si="0"/>
@@ -45202,7 +45224,7 @@
         <v>1040</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I67" s="5" t="str">
         <f t="shared" ref="I67:I69" si="1">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B67, "'", "''"), "', TO_DATE('", C67, "', 'MM/DD/YYYY'), TO_DATE('", D67, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E67, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F67, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A67, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G67, "'", "''"), "'), '", H67, "');")</f>
@@ -45232,7 +45254,7 @@
         <v>1040</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I68" s="5" t="str">
         <f t="shared" si="1"/>
@@ -45262,7 +45284,7 @@
         <v>1040</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I69" s="5" t="str">
         <f t="shared" si="1"/>
@@ -45301,7 +45323,7 @@
         <v>1040</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I72" s="5" t="str">
         <f t="shared" ref="I72:I78" si="2">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B72, "'", "''"), "', TO_DATE('", C72, "', 'MM/DD/YYYY'), TO_DATE('", D72, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E72, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F72, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A72, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G72, "'", "''"), "'), '", H72, "');")</f>
@@ -45331,7 +45353,7 @@
         <v>1040</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I73" s="5" t="str">
         <f t="shared" si="2"/>
@@ -45361,7 +45383,7 @@
         <v>1040</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I74" s="5" t="str">
         <f t="shared" si="2"/>
@@ -45391,7 +45413,7 @@
         <v>1040</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I75" s="5" t="str">
         <f t="shared" si="2"/>
@@ -45421,7 +45443,7 @@
         <v>1040</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I76" s="5" t="str">
         <f t="shared" si="2"/>
@@ -45451,7 +45473,7 @@
         <v>1040</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I77" s="5" t="str">
         <f t="shared" si="2"/>
@@ -45481,7 +45503,7 @@
         <v>1040</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I78" s="5" t="str">
         <f t="shared" si="2"/>
@@ -45511,7 +45533,7 @@
         <v>1040</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I81" s="5" t="str">
         <f>CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B81, "'", "''"), "', TO_DATE('", C81, "', 'MM/DD/YYYY'), TO_DATE('", D81, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E81, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F81, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A81, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G81, "'", "''"), "'), '", H81, "');")</f>
@@ -45520,7 +45542,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -45546,7 +45568,7 @@
         <v>1040</v>
       </c>
       <c r="H87" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I87" s="5" t="str">
         <f t="shared" ref="I87:I122" si="3">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B87, "'", "''"), "', TO_DATE('", C87, "', 'MM/DD/YYYY'), TO_DATE('", D87, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E87, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F87, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A87, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G87, "'", "''"), "'), '", H87, "');")</f>
@@ -45576,7 +45598,7 @@
         <v>1040</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I88" s="5" t="str">
         <f t="shared" si="3"/>
@@ -45605,12 +45627,12 @@
       <c r="G89" s="5" t="s">
         <v>1040</v>
       </c>
-      <c r="H89" s="6" t="s">
-        <v>2016</v>
+      <c r="H89" s="25" t="s">
+        <v>2132</v>
       </c>
       <c r="I89" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-21-01 Leg 1', TO_DATE('10/15/2020', 'MM/DD/YYYY'), TO_DATE('10/30/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-21-01 Leg 1', TO_DATE('10/15/2020', 'MM/DD/YYYY'), TO_DATE('10/30/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-21-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'IDK What is this field?');</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -45636,7 +45658,7 @@
         <v>1040</v>
       </c>
       <c r="H90" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I90" s="5" t="str">
         <f t="shared" si="3"/>
@@ -45666,7 +45688,7 @@
         <v>1040</v>
       </c>
       <c r="H91" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I91" s="5" t="str">
         <f t="shared" si="3"/>
@@ -45696,7 +45718,7 @@
         <v>1040</v>
       </c>
       <c r="H92" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I92" s="5" t="str">
         <f t="shared" si="3"/>
@@ -45726,7 +45748,7 @@
         <v>1040</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I93" s="5" t="str">
         <f t="shared" si="3"/>
@@ -45756,7 +45778,7 @@
         <v>1040</v>
       </c>
       <c r="H94" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I94" s="5" t="str">
         <f t="shared" si="3"/>
@@ -45786,7 +45808,7 @@
         <v>1040</v>
       </c>
       <c r="H95" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I95" s="5" t="str">
         <f t="shared" si="3"/>
@@ -45816,7 +45838,7 @@
         <v>1040</v>
       </c>
       <c r="H96" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I96" s="5" t="str">
         <f t="shared" si="3"/>
@@ -45846,7 +45868,7 @@
         <v>1040</v>
       </c>
       <c r="H97" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I97" s="5" t="str">
         <f t="shared" si="3"/>
@@ -45876,7 +45898,7 @@
         <v>1040</v>
       </c>
       <c r="H98" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I98" s="5" t="str">
         <f t="shared" si="3"/>
@@ -45905,12 +45927,12 @@
       <c r="G99" s="5" t="s">
         <v>1040</v>
       </c>
-      <c r="H99" s="6" t="s">
-        <v>2016</v>
+      <c r="H99" s="25" t="s">
+        <v>2131</v>
       </c>
       <c r="I99" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI-20-08 Leg 1', TO_DATE('6/10/2020', 'MM/DD/YYYY'), TO_DATE('6/29/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI-20-08 Leg 1', TO_DATE('6/10/2020', 'MM/DD/YYYY'), TO_DATE('6/29/2020', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (remove cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI-20-08'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Something else');</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -45936,7 +45958,7 @@
         <v>1040</v>
       </c>
       <c r="H100" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I100" s="5" t="str">
         <f t="shared" si="3"/>
@@ -45966,7 +45988,7 @@
         <v>1040</v>
       </c>
       <c r="H101" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I101" s="5" t="str">
         <f t="shared" si="3"/>
@@ -45996,7 +46018,7 @@
         <v>1040</v>
       </c>
       <c r="H102" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I102" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46026,7 +46048,7 @@
         <v>1040</v>
       </c>
       <c r="H103" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I103" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46056,7 +46078,7 @@
         <v>1040</v>
       </c>
       <c r="H104" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I104" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46086,7 +46108,7 @@
         <v>1040</v>
       </c>
       <c r="H105" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I105" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46116,7 +46138,7 @@
         <v>1040</v>
       </c>
       <c r="H106" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I106" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46146,7 +46168,7 @@
         <v>1040</v>
       </c>
       <c r="H107" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I107" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46176,7 +46198,7 @@
         <v>1040</v>
       </c>
       <c r="H108" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I108" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46206,7 +46228,7 @@
         <v>1040</v>
       </c>
       <c r="H109" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I109" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46236,7 +46258,7 @@
         <v>1040</v>
       </c>
       <c r="H110" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I110" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46266,7 +46288,7 @@
         <v>1040</v>
       </c>
       <c r="H111" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I111" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46295,12 +46317,12 @@
       <c r="G112" s="5" t="s">
         <v>1040</v>
       </c>
-      <c r="H112" s="6" t="s">
-        <v>2016</v>
+      <c r="H112" s="25" t="s">
+        <v>2130</v>
       </c>
       <c r="I112" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-19-04 Leg 2', TO_DATE('6/19/2019', 'MM/DD/YYYY'), TO_DATE('7/12/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-04'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-19-04 Leg 2', TO_DATE('6/19/2019', 'MM/DD/YYYY'), TO_DATE('7/12/2019', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 2)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-19-04'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Mountain/Pacific Time');</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
@@ -46326,7 +46348,7 @@
         <v>1040</v>
       </c>
       <c r="H113" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I113" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46356,7 +46378,7 @@
         <v>1040</v>
       </c>
       <c r="H114" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I114" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46386,7 +46408,7 @@
         <v>1040</v>
       </c>
       <c r="H115" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I115" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46416,7 +46438,7 @@
         <v>1040</v>
       </c>
       <c r="H116" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I116" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46446,7 +46468,7 @@
         <v>1040</v>
       </c>
       <c r="H117" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I117" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46476,7 +46498,7 @@
         <v>1040</v>
       </c>
       <c r="H118" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I118" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46506,7 +46528,7 @@
         <v>1040</v>
       </c>
       <c r="H119" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I119" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46535,12 +46557,12 @@
       <c r="G120" s="5" t="s">
         <v>1040</v>
       </c>
-      <c r="H120" s="6" t="s">
-        <v>2016</v>
+      <c r="H120" s="25" t="s">
+        <v>2129</v>
       </c>
       <c r="I120" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-22-01 Leg 2', TO_DATE('11/15/2021', 'MM/DD/YYYY'), TO_DATE('12/4/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('SE-22-01 Leg 2', TO_DATE('11/15/2021', 'MM/DD/YYYY'), TO_DATE('12/4/2021', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes (update cruise leg test case 4)', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'SE-22-01'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Eastern US Time');</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
@@ -46566,7 +46588,7 @@
         <v>1040</v>
       </c>
       <c r="H121" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I121" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46596,7 +46618,7 @@
         <v>1040</v>
       </c>
       <c r="H122" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I122" s="5" t="str">
         <f t="shared" si="3"/>
@@ -46605,7 +46627,7 @@
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
@@ -46616,13 +46638,13 @@
         <v>327</v>
       </c>
       <c r="C126" s="20" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="D126" s="20" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="E126" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F126" t="s">
         <v>94</v>
@@ -46631,7 +46653,7 @@
         <v>1040</v>
       </c>
       <c r="H126" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I126" s="5" t="str">
         <f t="shared" ref="I126:I153" si="4">CONCATENATE("insert into ccd_cruise_legs (", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ", ", F$1, ", ", A$1, ", ", G$1, ", ", H$1, ") values ('", SUBSTITUTE(B126, "'", "''"), "', TO_DATE('", C126, "', 'MM/DD/YYYY'), TO_DATE('", D126, "', 'MM/DD/YYYY'), '", SUBSTITUTE(E126, "'", "''"), "', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = '", F126, "'), (select vessel_id from ccd_vessels where vessel_name = '", SUBSTITUTE(A126, "'", "''"), "'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = '", SUBSTITUTE(G126, "'", "''"), "'), '", H126, "');")</f>
@@ -46648,13 +46670,13 @@
         <v>95</v>
       </c>
       <c r="C127" s="20" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="D127" s="20" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
       <c r="E127" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F127" t="s">
         <v>94</v>
@@ -46663,7 +46685,7 @@
         <v>1040</v>
       </c>
       <c r="H127" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I127" s="5" t="str">
         <f t="shared" si="4"/>
@@ -46680,13 +46702,13 @@
         <v>1862</v>
       </c>
       <c r="C128" s="20" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="D128" s="20" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="E128" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F128" t="s">
         <v>1862</v>
@@ -46695,7 +46717,7 @@
         <v>1040</v>
       </c>
       <c r="H128" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I128" s="5" t="str">
         <f t="shared" si="4"/>
@@ -46712,13 +46734,13 @@
         <v>260</v>
       </c>
       <c r="C129" s="20" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="D129" s="20" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="E129" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F129" t="s">
         <v>40</v>
@@ -46727,7 +46749,7 @@
         <v>1040</v>
       </c>
       <c r="H129" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I129" s="5" t="str">
         <f t="shared" si="4"/>
@@ -46744,13 +46766,13 @@
         <v>10</v>
       </c>
       <c r="C130" s="20" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="D130" s="20" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="E130" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F130" t="s">
         <v>10</v>
@@ -46759,7 +46781,7 @@
         <v>1040</v>
       </c>
       <c r="H130" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I130" s="5" t="str">
         <f t="shared" si="4"/>
@@ -46776,13 +46798,13 @@
         <v>47</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="D131" s="20" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="E131" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F131" t="s">
         <v>47</v>
@@ -46791,14 +46813,14 @@
         <v>1040</v>
       </c>
       <c r="H131" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I131" s="5" t="str">
         <f t="shared" si="4"/>
         <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0509', TO_DATE('07/19/2005', 'MM/DD/YYYY'), TO_DATE('08/05/2005', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0509'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
       </c>
       <c r="J131" s="24" t="s">
-        <v>2125</v>
+        <v>2124</v>
       </c>
       <c r="K131" s="19"/>
     </row>
@@ -46810,13 +46832,13 @@
         <v>261</v>
       </c>
       <c r="C132" s="20" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="D132" s="20" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="E132" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F132" t="s">
         <v>40</v>
@@ -46824,12 +46846,12 @@
       <c r="G132" s="5" t="s">
         <v>1040</v>
       </c>
-      <c r="H132" s="6" t="s">
-        <v>2016</v>
+      <c r="H132" s="25" t="s">
+        <v>2128</v>
       </c>
       <c r="I132" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0411_LEGII', TO_DATE('09/08/2005', 'MM/DD/YYYY'), TO_DATE('09/13/2005', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0411'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('OES0411_LEGII', TO_DATE('09/08/2005', 'MM/DD/YYYY'), TO_DATE('09/13/2005', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'OES0411'), (select vessel_id from ccd_vessels where vessel_name = 'Oscar Elton Sette'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'Hawaii Standard Time');</v>
       </c>
       <c r="J132" s="19"/>
       <c r="K132" s="19"/>
@@ -46842,13 +46864,13 @@
         <v>59</v>
       </c>
       <c r="C133" s="20" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="D133" s="20" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="E133" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F133" t="s">
         <v>59</v>
@@ -46857,7 +46879,7 @@
         <v>1040</v>
       </c>
       <c r="H133" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I133" s="5" t="str">
         <f t="shared" si="4"/>
@@ -46871,16 +46893,16 @@
         <v>4</v>
       </c>
       <c r="B134" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="C134" s="20" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="D134" s="20" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="E134" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F134" t="s">
         <v>15</v>
@@ -46889,7 +46911,7 @@
         <v>1040</v>
       </c>
       <c r="H134" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I134" s="5" t="str">
         <f t="shared" si="4"/>
@@ -46906,13 +46928,13 @@
         <v>65</v>
       </c>
       <c r="C135" s="20" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="D135" s="20" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="E135" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F135" t="s">
         <v>65</v>
@@ -46921,7 +46943,7 @@
         <v>1040</v>
       </c>
       <c r="H135" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I135" s="5" t="str">
         <f t="shared" si="4"/>
@@ -46938,13 +46960,13 @@
         <v>19</v>
       </c>
       <c r="C136" s="20" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="D136" s="20" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="E136" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F136" t="s">
         <v>18</v>
@@ -46953,7 +46975,7 @@
         <v>1040</v>
       </c>
       <c r="H136" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I136" s="5" t="str">
         <f t="shared" si="4"/>
@@ -46970,13 +46992,13 @@
         <v>20</v>
       </c>
       <c r="C137" s="20" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="D137" s="20" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="E137" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F137" t="s">
         <v>18</v>
@@ -46984,12 +47006,12 @@
       <c r="G137" s="5" t="s">
         <v>1040</v>
       </c>
-      <c r="H137" s="6" t="s">
-        <v>2016</v>
+      <c r="H137" s="25" t="s">
+        <v>2126</v>
       </c>
       <c r="I137" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI1001_LEGII', TO_DATE('03/21/2010', 'MM/DD/YYYY'), TO_DATE('06/30/2010', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1001'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('HI1001_LEGII', TO_DATE('03/21/2010', 'MM/DD/YYYY'), TO_DATE('06/30/2010', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'HI1001'), (select vessel_id from ccd_vessels where vessel_name = 'Hi''ialakai'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'ASDF JKL;');</v>
       </c>
       <c r="J137" s="19"/>
       <c r="K137" s="19"/>
@@ -47002,13 +47024,13 @@
         <v>21</v>
       </c>
       <c r="C138" s="20" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="D138" s="20" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="E138" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F138" t="s">
         <v>18</v>
@@ -47017,7 +47039,7 @@
         <v>1040</v>
       </c>
       <c r="H138" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I138" s="5" t="str">
         <f t="shared" si="4"/>
@@ -47034,13 +47056,13 @@
         <v>3</v>
       </c>
       <c r="C139" s="20" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="D139" s="20" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E139" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F139" t="s">
         <v>3</v>
@@ -47049,7 +47071,7 @@
         <v>1040</v>
       </c>
       <c r="H139" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I139" s="5" t="str">
         <f t="shared" si="4"/>
@@ -47066,13 +47088,13 @@
         <v>1863</v>
       </c>
       <c r="C140" s="20" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="D140" s="20" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E140" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F140" t="s">
         <v>1863</v>
@@ -47081,7 +47103,7 @@
         <v>1040</v>
       </c>
       <c r="H140" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I140" s="5" t="str">
         <f t="shared" si="4"/>
@@ -47098,13 +47120,13 @@
         <v>187</v>
       </c>
       <c r="C141" s="20" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="D141" s="20" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="E141" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F141" t="s">
         <v>23</v>
@@ -47113,7 +47135,7 @@
         <v>1040</v>
       </c>
       <c r="H141" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I141" s="5" t="str">
         <f t="shared" si="4"/>
@@ -47130,13 +47152,13 @@
         <v>324</v>
       </c>
       <c r="C142" s="20" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="D142" s="20" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
       <c r="E142" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F142" t="s">
         <v>23</v>
@@ -47145,7 +47167,7 @@
         <v>1040</v>
       </c>
       <c r="H142" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I142" s="5" t="str">
         <f t="shared" si="4"/>
@@ -47162,13 +47184,13 @@
         <v>325</v>
       </c>
       <c r="C143" s="20" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="D143" s="20" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="E143" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F143" t="s">
         <v>23</v>
@@ -47177,7 +47199,7 @@
         <v>1040</v>
       </c>
       <c r="H143" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I143" s="5" t="str">
         <f t="shared" si="4"/>
@@ -47194,22 +47216,22 @@
         <v>1869</v>
       </c>
       <c r="C144" s="20" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="D144" s="20" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
       <c r="E144" t="s">
+        <v>2059</v>
+      </c>
+      <c r="F144" t="s">
         <v>2060</v>
-      </c>
-      <c r="F144" t="s">
-        <v>2061</v>
       </c>
       <c r="G144" s="5" t="s">
         <v>1040</v>
       </c>
       <c r="H144" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I144" s="5" t="str">
         <f t="shared" si="4"/>
@@ -47226,22 +47248,22 @@
         <v>1870</v>
       </c>
       <c r="C145" s="20" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="D145" s="20" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
       <c r="E145" t="s">
+        <v>2059</v>
+      </c>
+      <c r="F145" t="s">
         <v>2060</v>
-      </c>
-      <c r="F145" t="s">
-        <v>2061</v>
       </c>
       <c r="G145" s="5" t="s">
         <v>1040</v>
       </c>
       <c r="H145" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I145" s="5" t="str">
         <f t="shared" si="4"/>
@@ -47258,13 +47280,13 @@
         <v>1867</v>
       </c>
       <c r="C146" s="20" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="D146" s="20" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="E146" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F146" t="s">
         <v>75</v>
@@ -47273,7 +47295,7 @@
         <v>1040</v>
       </c>
       <c r="H146" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I146" s="5" t="str">
         <f t="shared" si="4"/>
@@ -47290,13 +47312,13 @@
         <v>1868</v>
       </c>
       <c r="C147" s="20" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="D147" s="20" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="E147" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F147" t="s">
         <v>75</v>
@@ -47305,7 +47327,7 @@
         <v>1040</v>
       </c>
       <c r="H147" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I147" s="5" t="str">
         <f t="shared" si="4"/>
@@ -47322,13 +47344,13 @@
         <v>337</v>
       </c>
       <c r="C148" s="20" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="D148" s="20" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="E148" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F148" t="s">
         <v>333</v>
@@ -47337,7 +47359,7 @@
         <v>1040</v>
       </c>
       <c r="H148" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I148" s="5" t="str">
         <f t="shared" si="4"/>
@@ -47354,13 +47376,13 @@
         <v>338</v>
       </c>
       <c r="C149" s="20" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="D149" s="20" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="E149" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F149" t="s">
         <v>333</v>
@@ -47368,12 +47390,12 @@
       <c r="G149" s="5" t="s">
         <v>1040</v>
       </c>
-      <c r="H149" s="6" t="s">
-        <v>2016</v>
+      <c r="H149" s="25" t="s">
+        <v>2127</v>
       </c>
       <c r="I149" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('RL-17-05 Leg 2', TO_DATE('09/11/2017', 'MM/DD/YYYY'), TO_DATE('09/30/2017', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), 'US/Hawaii');</v>
+        <v>insert into ccd_cruise_legs (LEG_NAME, LEG_START_DATE, LEG_END_DATE, LEG_DESC, CRUISE_ID, VESSEL_ID, PLAT_TYPE_ID, TZ_NAME) values ('RL-17-05 Leg 2', TO_DATE('09/11/2017', 'MM/DD/YYYY'), TO_DATE('09/30/2017', 'MM/DD/YYYY'), 'Legs were fabricated for testing purposes', (SELECT CCD_CRUISES.CRUISE_ID FROM CCD_CRUISES where cruise_name = 'RL-17-05'), (select vessel_id from ccd_vessels where vessel_name = 'Reuben Lasker'), (select PLAT_TYPE_ID from CCD_PLAT_TYPES where PLAT_TYPE_NAME = 'Fishery Survey Vessel (FSV)'), '+09:00');</v>
       </c>
       <c r="J149" s="19"/>
       <c r="K149" s="19"/>
@@ -47386,13 +47408,13 @@
         <v>339</v>
       </c>
       <c r="C150" s="20" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="D150" s="20" t="s">
         <v>357</v>
       </c>
       <c r="E150" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F150" t="s">
         <v>333</v>
@@ -47401,7 +47423,7 @@
         <v>1040</v>
       </c>
       <c r="H150" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I150" s="5" t="str">
         <f t="shared" si="4"/>
@@ -47421,10 +47443,10 @@
         <v>349</v>
       </c>
       <c r="D151" s="20" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="E151" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F151" t="s">
         <v>333</v>
@@ -47433,7 +47455,7 @@
         <v>1040</v>
       </c>
       <c r="H151" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I151" s="5" t="str">
         <f t="shared" si="4"/>
@@ -47453,10 +47475,10 @@
         <v>350</v>
       </c>
       <c r="D152" s="20" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
       <c r="E152" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F152" t="s">
         <v>333</v>
@@ -47465,7 +47487,7 @@
         <v>1040</v>
       </c>
       <c r="H152" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I152" s="5" t="str">
         <f t="shared" si="4"/>
@@ -47482,13 +47504,13 @@
         <v>2007</v>
       </c>
       <c r="C153" s="20" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="D153" s="20" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="E153" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F153" t="s">
         <v>333</v>
@@ -47497,7 +47519,7 @@
         <v>1040</v>
       </c>
       <c r="H153" s="6" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="I153" s="5" t="str">
         <f t="shared" si="4"/>
@@ -55654,7 +55676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
@@ -55671,7 +55693,7 @@
         <v>323</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="C1" t="s">
         <v>109</v>
@@ -55682,7 +55704,7 @@
         <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="C2" s="5" t="str">
         <f t="shared" ref="C2" si="0">CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A2, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B2, "'));")</f>
@@ -55694,7 +55716,7 @@
         <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="C3" s="5" t="str">
         <f t="shared" ref="C3:C10" si="1">CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A3, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B3, "'));")</f>
@@ -55706,7 +55728,7 @@
         <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="C4" s="5" t="str">
         <f t="shared" si="1"/>
@@ -55718,7 +55740,7 @@
         <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="C5" s="5" t="str">
         <f t="shared" si="1"/>
@@ -55730,7 +55752,7 @@
         <v>139</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C6" s="5" t="str">
         <f t="shared" si="1"/>
@@ -55742,7 +55764,7 @@
         <v>139</v>
       </c>
       <c r="B7" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="C7" s="5" t="str">
         <f t="shared" si="1"/>
@@ -55754,7 +55776,7 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="C8" s="5" t="str">
         <f t="shared" si="1"/>
@@ -55766,7 +55788,7 @@
         <v>145</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C9" s="5" t="str">
         <f t="shared" si="1"/>
@@ -55778,7 +55800,7 @@
         <v>147</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C10" s="5" t="str">
         <f t="shared" si="1"/>
@@ -55790,7 +55812,7 @@
         <v>2008</v>
       </c>
       <c r="B11" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="C11" s="5" t="str">
         <f t="shared" ref="C11:C12" si="2">CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A11, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B11, "'));")</f>
@@ -55802,7 +55824,7 @@
         <v>2008</v>
       </c>
       <c r="B12" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="C12" s="5" t="str">
         <f t="shared" si="2"/>
@@ -55811,10 +55833,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="D24" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -55822,7 +55844,7 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="C25" s="5" t="str">
         <f>CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A25, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B25, "'));")</f>
@@ -55834,7 +55856,7 @@
         <v>1863</v>
       </c>
       <c r="B26" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="C26" s="5" t="str">
         <f>CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A26, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B26, "'));")</f>
@@ -55846,7 +55868,7 @@
         <v>187</v>
       </c>
       <c r="B27" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="C27" s="5" t="str">
         <f>CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A27, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B27, "'));")</f>
@@ -55858,7 +55880,7 @@
         <v>187</v>
       </c>
       <c r="B28" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="C28" s="5" t="str">
         <f t="shared" ref="C28:C29" si="3">CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A28, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B28, "'));")</f>
@@ -55870,7 +55892,7 @@
         <v>187</v>
       </c>
       <c r="B29" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
       <c r="C29" s="5" t="str">
         <f t="shared" si="3"/>
@@ -55882,7 +55904,7 @@
         <v>324</v>
       </c>
       <c r="B30" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="C30" s="5" t="str">
         <f>CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A30, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B30, "'));")</f>
@@ -55896,7 +55918,7 @@
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
       <c r="D31" s="23" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -55904,7 +55926,7 @@
         <v>1869</v>
       </c>
       <c r="B32" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="C32" s="5" t="str">
         <f t="shared" ref="C32:C44" si="4">CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A32, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B32, "'));")</f>
@@ -55916,7 +55938,7 @@
         <v>1869</v>
       </c>
       <c r="B33" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="C33" s="5" t="str">
         <f t="shared" si="4"/>
@@ -55928,7 +55950,7 @@
         <v>1869</v>
       </c>
       <c r="B34" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
       <c r="C34" s="5" t="str">
         <f t="shared" si="4"/>
@@ -55940,7 +55962,7 @@
         <v>1870</v>
       </c>
       <c r="B35" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="C35" s="5" t="str">
         <f t="shared" si="4"/>
@@ -55952,7 +55974,7 @@
         <v>1870</v>
       </c>
       <c r="B36" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="C36" s="5" t="str">
         <f t="shared" si="4"/>
@@ -55964,7 +55986,7 @@
         <v>1870</v>
       </c>
       <c r="B37" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="C37" s="5" t="str">
         <f t="shared" si="4"/>
@@ -55976,7 +55998,7 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="C38" s="5" t="str">
         <f t="shared" si="4"/>
@@ -55985,10 +56007,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="B39" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="C39" s="5" t="str">
         <f t="shared" si="4"/>
@@ -56000,7 +56022,7 @@
         <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="C40" s="5" t="str">
         <f t="shared" si="4"/>
@@ -56012,7 +56034,7 @@
         <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="C41" s="5" t="str">
         <f t="shared" si="4"/>
@@ -56024,7 +56046,7 @@
         <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="C42" s="5" t="str">
         <f t="shared" si="4"/>
@@ -56036,7 +56058,7 @@
         <v>260</v>
       </c>
       <c r="B43" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="C43" s="5" t="str">
         <f t="shared" si="4"/>
@@ -56048,7 +56070,7 @@
         <v>261</v>
       </c>
       <c r="B44" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="C44" s="5" t="str">
         <f t="shared" si="4"/>
@@ -56062,7 +56084,7 @@
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
       <c r="D45" s="18" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -56070,7 +56092,7 @@
         <v>59</v>
       </c>
       <c r="B46" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="C46" s="5" t="str">
         <f>CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A46, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B46, "'));")</f>
@@ -56082,7 +56104,7 @@
         <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="C47" s="5" t="str">
         <f>CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A47, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B47, "'));")</f>
@@ -56094,7 +56116,7 @@
         <v>337</v>
       </c>
       <c r="B48" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C48" s="5" t="str">
         <f>CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A48, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B48, "'));")</f>
@@ -56106,7 +56128,7 @@
         <v>338</v>
       </c>
       <c r="B49" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C49" s="5" t="str">
         <f>CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A49, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B49, "'));")</f>
@@ -56120,7 +56142,7 @@
       <c r="B50" s="18"/>
       <c r="C50" s="18"/>
       <c r="D50" s="18" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -56128,7 +56150,7 @@
         <v>340</v>
       </c>
       <c r="B51" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C51" s="5" t="str">
         <f>CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A51, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B51, "'));")</f>
@@ -56140,7 +56162,7 @@
         <v>341</v>
       </c>
       <c r="B52" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C52" s="5" t="str">
         <f>CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A52, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B52, "'));")</f>
@@ -56152,7 +56174,7 @@
         <v>2007</v>
       </c>
       <c r="B53" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C53" s="5" t="str">
         <f>CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A53, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B53, "'));")</f>
@@ -56164,7 +56186,7 @@
         <v>1867</v>
       </c>
       <c r="B54" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="C54" s="5" t="str">
         <f>CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A54, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B54, "'));")</f>
@@ -56176,7 +56198,7 @@
         <v>1867</v>
       </c>
       <c r="B55" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="C55" s="5" t="str">
         <f t="shared" ref="C55:C59" si="5">CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A55, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B55, "'));")</f>
@@ -56188,7 +56210,7 @@
         <v>1867</v>
       </c>
       <c r="B56" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="C56" s="5" t="str">
         <f t="shared" si="5"/>
@@ -56200,7 +56222,7 @@
         <v>1868</v>
       </c>
       <c r="B57" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="C57" s="5" t="str">
         <f t="shared" si="5"/>
@@ -56212,7 +56234,7 @@
         <v>1868</v>
       </c>
       <c r="B58" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="C58" s="5" t="str">
         <f t="shared" si="5"/>
@@ -56224,7 +56246,7 @@
         <v>1868</v>
       </c>
       <c r="B59" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="C59" s="5" t="str">
         <f t="shared" si="5"/>
@@ -56238,7 +56260,7 @@
       <c r="B60" s="18"/>
       <c r="C60" s="18"/>
       <c r="D60" s="18" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -56246,7 +56268,7 @@
         <v>95</v>
       </c>
       <c r="B61" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="C61" s="5" t="str">
         <f>CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A61, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B61, "'));")</f>
@@ -56258,7 +56280,7 @@
         <v>1862</v>
       </c>
       <c r="B62" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="C62" s="5" t="str">
         <f>CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A62, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B62, "'));")</f>
@@ -56267,7 +56289,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="67" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -56275,10 +56297,10 @@
         <v>1875</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -56286,10 +56308,10 @@
         <v>1893</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D68" s="17" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -56297,7 +56319,7 @@
         <v>1877</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C69" s="9" t="str">
         <f t="shared" ref="C69:C112" si="6">CONCATENATE("insert into ccd_leg_data_sets (cruise_leg_id, DATA_SET_ID) values ((select cruise_leg_id from ccd_cruise_legs where leg_name = '", A69, "'), (SELECT DATA_SET_ID FROM CCD_DATA_SETS WHERE DATA_SET_NAME = '", B69, "'));")</f>
@@ -56309,7 +56331,7 @@
         <v>1877</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="C70" s="9" t="str">
         <f t="shared" si="6"/>
@@ -56321,7 +56343,7 @@
         <v>1878</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C71" s="9" t="str">
         <f t="shared" si="6"/>
@@ -56333,7 +56355,7 @@
         <v>1878</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="C72" s="9" t="str">
         <f t="shared" si="6"/>
@@ -56345,10 +56367,10 @@
         <v>1879</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -56356,7 +56378,7 @@
         <v>1880</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C74" s="9" t="str">
         <f t="shared" si="6"/>
@@ -56368,7 +56390,7 @@
         <v>1881</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C75" s="9" t="str">
         <f t="shared" si="6"/>
@@ -56380,7 +56402,7 @@
         <v>1882</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="C76" s="9" t="str">
         <f t="shared" si="6"/>
@@ -56392,7 +56414,7 @@
         <v>1882</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="C77" s="9" t="str">
         <f t="shared" si="6"/>
@@ -56404,7 +56426,7 @@
         <v>1882</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C78" s="9" t="str">
         <f t="shared" si="6"/>
@@ -56416,7 +56438,7 @@
         <v>1883</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="C79" s="9" t="str">
         <f t="shared" si="6"/>
@@ -56428,7 +56450,7 @@
         <v>1884</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C80" s="9" t="str">
         <f t="shared" si="6"/>
@@ -56440,10 +56462,10 @@
         <v>1890</v>
       </c>
       <c r="B81" s="17" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="82" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -56451,7 +56473,7 @@
         <v>1891</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C82" s="9" t="str">
         <f t="shared" si="6"/>
@@ -56463,7 +56485,7 @@
         <v>1920</v>
       </c>
       <c r="B83" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="C83" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56475,7 +56497,7 @@
         <v>1920</v>
       </c>
       <c r="B84" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="C84" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56487,7 +56509,7 @@
         <v>1920</v>
       </c>
       <c r="B85" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="C85" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56499,7 +56521,7 @@
         <v>1921</v>
       </c>
       <c r="B86" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="C86" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56511,7 +56533,7 @@
         <v>1921</v>
       </c>
       <c r="B87" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="C87" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56523,7 +56545,7 @@
         <v>1921</v>
       </c>
       <c r="B88" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="C88" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56535,7 +56557,7 @@
         <v>1922</v>
       </c>
       <c r="B89" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="C89" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56547,7 +56569,7 @@
         <v>1923</v>
       </c>
       <c r="B90" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="C90" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56559,7 +56581,7 @@
         <v>1924</v>
       </c>
       <c r="D91" s="17" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -56567,7 +56589,7 @@
         <v>1938</v>
       </c>
       <c r="B92" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="C92" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56579,7 +56601,7 @@
         <v>1939</v>
       </c>
       <c r="B93" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="C93" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56591,7 +56613,7 @@
         <v>1940</v>
       </c>
       <c r="B94" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="C94" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56603,7 +56625,7 @@
         <v>1940</v>
       </c>
       <c r="B95" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="C95" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56615,7 +56637,7 @@
         <v>1941</v>
       </c>
       <c r="B96" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="C96" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56627,7 +56649,7 @@
         <v>1942</v>
       </c>
       <c r="B97" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="C97" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56639,7 +56661,7 @@
         <v>1942</v>
       </c>
       <c r="B98" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="C98" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56651,7 +56673,7 @@
         <v>1945</v>
       </c>
       <c r="B99" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="C99" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56663,7 +56685,7 @@
         <v>1947</v>
       </c>
       <c r="B100" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="C100" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56675,7 +56697,7 @@
         <v>1978</v>
       </c>
       <c r="B101" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="C101" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56687,7 +56709,7 @@
         <v>1979</v>
       </c>
       <c r="B102" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="C102" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56699,7 +56721,7 @@
         <v>1980</v>
       </c>
       <c r="B103" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="C103" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56711,7 +56733,7 @@
         <v>1981</v>
       </c>
       <c r="B104" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="C104" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56723,7 +56745,7 @@
         <v>1963</v>
       </c>
       <c r="B105" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="C105" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56735,7 +56757,7 @@
         <v>1974</v>
       </c>
       <c r="B106" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="C106" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56747,7 +56769,7 @@
         <v>1964</v>
       </c>
       <c r="D107" s="18" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -56755,7 +56777,7 @@
         <v>1965</v>
       </c>
       <c r="B108" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="C108" s="5" t="str">
         <f t="shared" si="6"/>
@@ -56767,7 +56789,7 @@
         <v>2005</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="C109" s="9" t="str">
         <f t="shared" si="6"/>
@@ -56779,7 +56801,7 @@
         <v>2006</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="C110" s="9" t="str">
         <f t="shared" si="6"/>
@@ -56791,7 +56813,7 @@
         <v>1994</v>
       </c>
       <c r="D111" s="18" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="112" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -56799,7 +56821,7 @@
         <v>1993</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="C112" s="9" t="str">
         <f t="shared" si="6"/>
@@ -57482,7 +57504,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>136</v>
@@ -57491,7 +57513,7 @@
         <v>137</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>176</v>
@@ -57502,10 +57524,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C2" t="s">
         <v>110</v>
@@ -57523,10 +57545,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C3" t="s">
         <v>110</v>
@@ -57544,7 +57566,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" t="s">
@@ -57563,7 +57585,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="C5" t="s">
         <v>113</v>
@@ -57581,7 +57603,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="C6" t="s">
         <v>141</v>
@@ -57596,7 +57618,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="C7" t="s">
         <v>143</v>
@@ -57614,10 +57636,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C8" t="s">
         <v>110</v>
@@ -57632,10 +57654,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="B9" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C9" t="s">
         <v>110</v>
@@ -57653,7 +57675,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="C10" t="s">
         <v>111</v>
@@ -57668,7 +57690,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="C11" t="s">
         <v>111</v>
@@ -57683,7 +57705,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="C12" t="s">
         <v>111</v>
@@ -57698,7 +57720,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="C13" t="s">
         <v>111</v>
@@ -57713,7 +57735,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="C14" t="s">
         <v>111</v>
@@ -57770,12 +57792,12 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="C27" t="s">
         <v>111</v>
@@ -57790,7 +57812,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="C28" t="s">
         <v>111</v>
@@ -57805,7 +57827,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C29" t="s">
         <v>111</v>
@@ -57820,7 +57842,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="C30" t="s">
         <v>111</v>
@@ -57835,7 +57857,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="C31" t="s">
         <v>113</v>
@@ -57850,7 +57872,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="C32" t="s">
         <v>141</v>
@@ -57865,7 +57887,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="C33" t="s">
         <v>113</v>
@@ -57880,7 +57902,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="C34" t="s">
         <v>141</v>
@@ -57895,7 +57917,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="C35" t="s">
         <v>113</v>
@@ -57910,7 +57932,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="C36" t="s">
         <v>141</v>
@@ -57925,7 +57947,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="C37" t="s">
         <v>113</v>
@@ -57940,7 +57962,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="C38" t="s">
         <v>141</v>
@@ -57955,7 +57977,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="C39" t="s">
         <v>114</v>
@@ -57970,7 +57992,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="C40" t="s">
         <v>115</v>
@@ -57985,7 +58007,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="C41" t="s">
         <v>114</v>
@@ -58000,7 +58022,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="C42" t="s">
         <v>115</v>
@@ -58015,7 +58037,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="C43" t="s">
         <v>114</v>
@@ -58030,7 +58052,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="C44" t="s">
         <v>115</v>
@@ -58045,7 +58067,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="C45" t="s">
         <v>114</v>
@@ -58060,7 +58082,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="C46" t="s">
         <v>115</v>
@@ -58075,12 +58097,12 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="C52" t="s">
         <v>111</v>
@@ -58095,7 +58117,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="C53" t="s">
         <v>111</v>
@@ -58110,7 +58132,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="C54" t="s">
         <v>111</v>
@@ -58125,7 +58147,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="C55" t="s">
         <v>111</v>
@@ -58140,7 +58162,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="C56" t="s">
         <v>111</v>
@@ -58155,7 +58177,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="C57" t="s">
         <v>111</v>
@@ -58170,7 +58192,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="C58" t="s">
         <v>111</v>
@@ -58185,7 +58207,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="C59" t="s">
         <v>111</v>
@@ -58200,7 +58222,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="C60" t="s">
         <v>111</v>
@@ -58215,7 +58237,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="C61" t="s">
         <v>111</v>
@@ -58230,7 +58252,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C62" t="s">
         <v>111</v>
@@ -58245,7 +58267,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="C63" t="s">
         <v>141</v>
@@ -58260,7 +58282,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="C64" t="s">
         <v>113</v>
@@ -58275,7 +58297,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="C65" t="s">
         <v>115</v>
@@ -58290,7 +58312,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
       <c r="C66" t="s">
         <v>114</v>
@@ -58305,7 +58327,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="C67" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
bug fix for category 5
</commit_message>
<xml_diff>
--- a/docs/Cruise_Leg_DDL_DML_generator.xlsx
+++ b/docs/Cruise_Leg_DDL_DML_generator.xlsx
@@ -43374,8 +43374,8 @@
   <dimension ref="A1:K153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H89" sqref="H89"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I126" sqref="I126:I153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>